<commit_message>
update annotation results to add parent it
変更履歴の親注釈を返却できるようにした
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB3B4DF-D938-4793-8A75-B0E817DD2C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA11DDA2-B0B4-4BFD-AAA3-0E5777E490C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="18525" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="18780" windowWidth="28800" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="月" sheetId="3" r:id="rId1"/>
@@ -4252,7 +4252,7 @@
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.59765625" defaultRowHeight="20" customHeight="1"/>
@@ -4386,8 +4386,8 @@
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="4">
         <v>156</v>
@@ -26178,7 +26178,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
update gihou and daien operation
注記を加えた
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ty/ruby/zakuro/doc/operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195CD649-31B4-704B-92F8-D1CE2AA1222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{F957D327-49AD-5A40-BAE0-C484C5296427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20700" yWindow="-43200" windowWidth="35060" windowHeight="43200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="月" sheetId="3" r:id="rId1"/>
@@ -21,11 +21,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">月!$B$1:$AG$447</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7537" uniqueCount="1714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7680" uniqueCount="1780">
   <si>
     <t>ID</t>
   </si>
@@ -4851,15 +4852,9 @@
     <t>延暦 11年 2 大 丙戌 22-583</t>
   </si>
   <si>
-    <t>延暦 11年 3 小 丙辰 51-2238</t>
-  </si>
-  <si>
     <t>延暦 11年 9 大 癸丑 49-1025</t>
   </si>
   <si>
-    <t>延暦 11年 10 小 癸未 18-2659</t>
-  </si>
-  <si>
     <t>延暦 11年 11 大 壬子 48-1153</t>
   </si>
   <si>
@@ -4878,9 +4873,6 @@
     <t>延暦 14年 8 大 乙丑  1-897</t>
   </si>
   <si>
-    <t>延暦 14年 9 小 乙未  30-2999</t>
-  </si>
-  <si>
     <t>延暦 14年 12 大 甲子 0-953</t>
   </si>
   <si>
@@ -4890,30 +4882,18 @@
     <t>延暦 16年 9 大 癸未 19-1512</t>
   </si>
   <si>
-    <t>延暦 16年 10 小 癸丑 48-3021</t>
-  </si>
-  <si>
     <t>延暦 17年 1 大 壬午 18-445</t>
   </si>
   <si>
-    <t>延暦 17年 2 小 壬子 47-2780</t>
-  </si>
-  <si>
     <t>延暦 17年 10 大 丙子  12-2991</t>
   </si>
   <si>
     <t>延暦 17年 12 大 丙子 12-731</t>
   </si>
   <si>
-    <t>延暦 18年 1 小 丙午 41-2849</t>
-  </si>
-  <si>
     <t>延暦 18年 3 大 乙巳 41-1077</t>
   </si>
   <si>
-    <t>延暦 18年 4 小 乙亥  10-3034</t>
-  </si>
-  <si>
     <t>延暦 20年 6 大 辛卯 27-2957</t>
   </si>
   <si>
@@ -4926,54 +4906,36 @@
     <t>延暦 24年 12 大 丙申 32-385</t>
   </si>
   <si>
-    <t>大同 1年 1 小 丙寅 1-2844</t>
-  </si>
-  <si>
     <t>大同 1年 9 大 庚寅  26-2750</t>
   </si>
   <si>
     <t>大同 1年 11 大 庚寅 26-503</t>
   </si>
   <si>
-    <t>大同 1年 12 大 庚申 55-2820</t>
-  </si>
-  <si>
     <t>大同 2年 1 小 庚寅  25-2102</t>
   </si>
   <si>
     <t>大同 3年 5 大 壬午 18-1293</t>
   </si>
   <si>
-    <t>大同 3年 6 小 壬子  47-2842</t>
-  </si>
-  <si>
     <t>大同 3年 11 大 戊寅 14-2998</t>
   </si>
   <si>
     <t>弘仁 4年 7 大 辛亥 47-1494</t>
   </si>
   <si>
-    <t>弘仁 4年 8 小 辛巳 16-3026</t>
-  </si>
-  <si>
     <t>弘仁 6年 11 大 丁卯  3-2977</t>
   </si>
   <si>
     <t>弘仁 7年 11 大 壬戌  58-1048</t>
   </si>
   <si>
-    <t>弘仁 7年 12 小 壬辰  27-2812</t>
-  </si>
-  <si>
     <t>弘仁 8年 3 大 庚申 56-2880</t>
   </si>
   <si>
     <t>弘仁 8年 9 大 丁亥 23-1704</t>
   </si>
   <si>
-    <t>弘仁 8年 10 小 丁巳  52-2903</t>
-  </si>
-  <si>
     <t>弘仁 8年 12 大 乙卯 51-2878</t>
   </si>
   <si>
@@ -4983,30 +4945,15 @@
     <t>弘仁 9年 12 大 庚戌 46-1657</t>
   </si>
   <si>
-    <t>弘仁 10年 1 小 庚辰  15-3026</t>
-  </si>
-  <si>
     <t>弘仁 10年 2 大 己酉 45-1384</t>
   </si>
   <si>
-    <t>弘仁 10年 3 小 己卯 14-2828</t>
-  </si>
-  <si>
     <t>弘仁 11年 閏1 大 甲辰 40-222</t>
   </si>
   <si>
-    <t>弘仁 11年 2 小 甲戌  9-1402</t>
-  </si>
-  <si>
-    <t>弘仁 11年 3 小 癸卯  38-2626</t>
-  </si>
-  <si>
     <t>弘仁 11年 6 大 辛未  7-929</t>
   </si>
   <si>
-    <t>弘仁 11年 7 小 辛丑 36-2826</t>
-  </si>
-  <si>
     <t>弘仁 12年 7 大 乙未 31-184</t>
   </si>
   <si>
@@ -5019,9 +4966,6 @@
     <t>弘仁 13年 1 大 癸巳 29-802</t>
   </si>
   <si>
-    <t>弘仁 13年 2 小 癸亥 58-2380</t>
-  </si>
-  <si>
     <t>弘仁 14年 10 大 辛巳 17-2819</t>
   </si>
   <si>
@@ -5043,27 +4987,12 @@
     <t>天長 4年 12 大 戊子 24-1551</t>
   </si>
   <si>
-    <t>天長 5年 1 大 戊午 53-2901</t>
-  </si>
-  <si>
-    <t>天長 5年 2 小 戊子  23-1209</t>
-  </si>
-  <si>
-    <t>天長 5年 3 小 丁巳  52-2600</t>
-  </si>
-  <si>
     <t>天長 5年 9 大 癸未 19-2980</t>
   </si>
   <si>
     <t>天長 7年 5 大 甲戌  10-469</t>
   </si>
   <si>
-    <t>天長 7年 6 小 甲辰 39-1519</t>
-  </si>
-  <si>
-    <t>天長 7年 7 小 癸酉 8-2856</t>
-  </si>
-  <si>
     <t>天長 8年 9 大 乙未  31-2805</t>
   </si>
   <si>
@@ -5079,159 +5008,81 @@
     <t>承和 1年 12 大 丁丑 13-887</t>
   </si>
   <si>
-    <t>承和 2年 1 小 丁未 42-2793</t>
-  </si>
-  <si>
     <t>承和 3年 7 大 戊辰  4-1260</t>
   </si>
   <si>
-    <t>承和 3年 8 小 戊戌 33-2996</t>
-  </si>
-  <si>
     <t>承和 3年 9 大 丁卯  3-1517</t>
   </si>
   <si>
-    <t>承和 3年 10 小 丁酉 32-3000</t>
-  </si>
-  <si>
     <t>承和 5年 8 大 丙戌 22-658</t>
   </si>
   <si>
-    <t>承和 5年 9 小 丙辰 51-2800</t>
-  </si>
-  <si>
     <t>承和 6年 7 大 庚辰 16-1078</t>
   </si>
   <si>
-    <t>承和 6年 8 小 庚戌 45-2916</t>
-  </si>
-  <si>
     <t>承和 6年 11 大 己卯 15-600</t>
   </si>
   <si>
-    <t>承和 6年 12 小 己酉 44-2892</t>
-  </si>
-  <si>
     <t>承和 9年 2 大 丙寅 2-864</t>
   </si>
   <si>
-    <t>承和 9年 3 小 丙申 31-2738</t>
-  </si>
-  <si>
     <t>承和 9年 11 大 辛卯 27-518</t>
   </si>
   <si>
-    <t>承和 9年 12 小 辛酉 56-2661</t>
-  </si>
-  <si>
     <t>承和 11年 5 大 癸未 19-1172</t>
   </si>
   <si>
-    <t>承和 11年 6 小 癸丑 48-2934</t>
-  </si>
-  <si>
     <t>承和 11年 8 大 辛巳 17-1383</t>
   </si>
   <si>
-    <t>承和 11年 9 小 辛亥 46-2695</t>
-  </si>
-  <si>
     <t>承和 12年 9 大 乙巳 41-1264</t>
   </si>
   <si>
-    <t>承和 12年 10 小 乙亥 10-2799</t>
-  </si>
-  <si>
     <t>承和 12年 11 大 甲辰 40-1261</t>
   </si>
   <si>
-    <t>承和 12年 12 小 甲戌 9-2726</t>
-  </si>
-  <si>
     <t>承和 13年 10 大 己巳  5-937</t>
   </si>
   <si>
-    <t>承和 13年 11 小 己亥  34-2812</t>
-  </si>
-  <si>
     <t>承和 14年 4 大 乙未 31-1608</t>
   </si>
   <si>
-    <t>承和 14年 5 小 乙丑 0-2867</t>
-  </si>
-  <si>
     <t>承和 14年 10 大 癸巳 29-475</t>
   </si>
   <si>
-    <t>承和 14年 11 小 癸亥 58-2640</t>
-  </si>
-  <si>
     <t>嘉祥 1年 10 大 丁亥 23-564</t>
   </si>
   <si>
-    <t>嘉祥 1年 11 小 丁巳 52-2966</t>
-  </si>
-  <si>
     <t>嘉祥 2年 10 大 辛巳 17-744</t>
   </si>
   <si>
-    <t>嘉祥 2年 11 小 辛亥 46-2922</t>
-  </si>
-  <si>
     <t>嘉祥 3年 1 大 庚辰 16-942</t>
   </si>
   <si>
-    <t>嘉祥 3年 2 小 庚戌  45-2860</t>
-  </si>
-  <si>
     <t>仁寿 3年 6 大 庚申 56-1132</t>
   </si>
   <si>
-    <t>仁寿 3年 7 小 庚寅 25-2763</t>
-  </si>
-  <si>
     <t>斎衡 1年 11 大 壬午 18-1071</t>
   </si>
   <si>
-    <t>斎衡 1年 12 大 壬子 47-2602</t>
-  </si>
-  <si>
     <t>斎衡 2年 1 小 壬午 17-902</t>
   </si>
   <si>
-    <t>斎衡 2年 2 小 辛亥 46-2139</t>
-  </si>
-  <si>
     <t>斎衡 2年 11 大 丙午 42-1215</t>
   </si>
   <si>
-    <t>斎衡 2年 12 小 丙子 11-2894</t>
-  </si>
-  <si>
     <t>斎衡 3年 9 大 辛丑 37-683</t>
   </si>
   <si>
-    <t>斎衡 3年 10 小 辛未 6-2919</t>
-  </si>
-  <si>
     <t>斎衡 3年 12 大 庚午  6-1214</t>
   </si>
   <si>
-    <t>天安 1年 1 小 庚子 35-2985</t>
-  </si>
-  <si>
     <t>天安 1年 9 大 乙未 31-805</t>
   </si>
   <si>
-    <t>天安 1年 10 小 乙丑  0-2932</t>
-  </si>
-  <si>
     <t>天安 2年 1 大 甲午 30-893</t>
   </si>
   <si>
-    <t>天安 2年 2 小 甲子 59-2856</t>
-  </si>
-  <si>
     <t>貞観 1年 9 大 癸丑 49-1398</t>
   </si>
   <si>
@@ -5241,15 +5092,9 @@
     <t>貞観 2年 1 大 壬子 48-391</t>
   </si>
   <si>
-    <t>貞観 2年 2 小 壬午 17-2710</t>
-  </si>
-  <si>
     <t>貞観 2年 10 大 丁丑 13-1449</t>
   </si>
   <si>
-    <t>貞観 2年 閏10 大 丁未  42-2908</t>
-  </si>
-  <si>
     <t>貞観 2年 11 小 丁丑 12-1628</t>
   </si>
   <si>
@@ -5262,13 +5107,7 @@
     <t>貞観 3年 3 大 乙亥 11-976</t>
   </si>
   <si>
-    <t>貞観 3年 4 小 乙巳 40-2910</t>
-  </si>
-  <si>
     <t>貞観 3年 5 大 甲戌 10-1533</t>
-  </si>
-  <si>
-    <t>貞観 3年 6 小 甲辰 39-2990</t>
   </si>
   <si>
     <t>乙亥</t>
@@ -6661,6 +6500,1450 @@
     </rPh>
     <rPh sb="6" eb="7">
       <t xml:space="preserve">ニホンキ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では55己未, 続日本紀により庚申，したがって7月朔のユリウス暦日は8月5日。</t>
+    <rPh sb="6" eb="7">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">ニホンキ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">ニホン </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>延暦 11年 3 小 丙辰 51-2238</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では51乙卯であるが日本逸史2月の條に乙卯があるから丙辰とする。3月丙辰朔とすればそのユリウス暦日は3月28日となる。</t>
+    <rPh sb="6" eb="7">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">ニホンキ </t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t xml:space="preserve">ニホン </t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>シュウイテゥ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>シジテゥ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>サク9</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>延暦 11年 10 小 癸未 18-2659</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では18壬午，日本逸史により癸未，したがって10月朔のユリウス暦日は10月21日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では17辛巳，日本逸史により壬午，したがって閏11月朔のユリウス暦日は12月19日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ウルウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>延暦 14年 9 小 乙未  30-2999</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は30甲午，日本逸史により乙未，したがって9月朔日のユリウス暦日は10月18日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ジテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は29癸巳，日本逸史により甲午，したがって正月朔日のユリウス暦日は2月14日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>延暦 16年 10 小 癸丑 48-3021</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算A）では壬子であるがC）では癸丑とでる。日本逸史9月に壬子がある。したがって，進朔して癸丑とすべきである。10月癸丑朔なら，そのユリウス暦日は10月25日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>シンサク</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>_x0000__x0000__x0002_</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>_x0004__x001B__x0001__x0007_)</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>_x0002__x000B_9</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>延暦 17年 2 小 壬子 47-2780</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では47辛亥であるが日本逸史に壬子朔とある。したがって2月朔のユリウス暦日は2月21日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ニホn</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t xml:space="preserve">キ </t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>サク</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>延暦 18年 1 小 丙午 41-2849</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では41乙巳であるが日本後紀により丙午，したがって正月朔のユリウス暦日は2月10日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>延暦 18年 4 小 乙亥  10-3034</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では10甲戌であるが日本後紀により乙亥，したがって4月朔のユリウス暦日は5月10日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>大同 1年 1 小 丙寅 1-2844</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では1乙丑，日本後紀により丙寅，したがって正月朔のユリウス暦日は1月24日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>大同 1年 12 大 庚申 55-2820</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では55己未，日本逸史により庚申，したがって12月朔のユリウス暦日は1月13日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では25己丑，日本逸史により庚寅，したがって正月朔のユリウス暦日は2月12日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>大同 3年 6 小 壬子  47-2842</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では47辛亥，日本逸史により壬子，したがって6月朔のユリウス暦日は6月28日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 4年 8 小 辛巳 16-3026</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は16庚辰，逸史により辛巳，したがって，8月朔のユリウス暦日は8月30日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 7年 12 小 壬辰  27-2812</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では27辛卯，逸史により壬辰，したがって12月朔のユリウス暦日は12月23日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 8年 10 小 丁巳  52-2903</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では52丙辰，逸史により丁巳，したがって10月朔のユリウス暦日は11月13日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 10年 1 小 庚辰  15-3026</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では15己卯であるが，逸史に庚辰朔とある。したがって正月朔のユリウス暦日は1月30日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t xml:space="preserve">イツシ </t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>シジテゥ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>2021/07/26</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 10年 3 小 己卯 14-2828</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 11年 2 小 甲戌  9-1402</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では14戊寅であるが，逸史に己卯朔とある。したがって3月朔のユリウス暦日は3月30日。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では9癸酉であるが，逸史に甲戌朔とある。したがって2月朔のユリウス暦日は3月19日。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 11年 3 小 癸卯  38-2626</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では38壬寅であるが，4月壬申と2月甲戌より3月朔は癸卯と定まる。3月朔のユリウス暦日は4月17日。</t>
+    <rPh sb="23" eb="24">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>7/26</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>サダマル</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 11年 7 小 辛丑 36-2826</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では36庚子であるが，逸史に辛丑朔とある。したがって7月朔のユリウス暦日は8月13日。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>逸史巻29，9月乙未朔とある。9月乙未朔とすれば8月甲子朔はあり得ない。ユリウス暦日は9月1日となる。</t>
+    <rPh sb="10" eb="11">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>_x0000_
+_x0001_</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>_x0005__x0010__x0001_</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>_x0008__x0014__x0001__x000B__x0019_</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>_x0001__x000E__x001A__x0002__x0013_</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t xml:space="preserve">_x001C__x0001__x0018_ </t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>_x0001__x001C_,</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>逸史巻29，9月乙未朔とある。したがって9月朔日のユリウス暦日は10月1日。</t>
+    <rPh sb="10" eb="11">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>_x0000_
+_x0001_</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>_x0005__x0010__x0001_</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>_x0008__x0017__x0001_</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>_x000B__x001A__x0001__x000E__x001B_</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>_x0002__x0013__x001D__x0001__x0018_</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>"_x0001__x001C_-_x0001__x001F_/</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>弘仁 13年 2 小 癸亥 58-2380</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>逸史に正月戊辰朔と計算より1日退いている。したがってユリウス暦日は2月10日。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天長 5年 1 大 戊午 53-2901</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天長 5年 2 小 戊子  23-1209</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では53丁巳であるが，逸史に戊午朔とある。したがって正月朔のユリウス暦日は1月21日となる。</t>
+    <rPh sb="26" eb="28">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では23丁亥であるが，逸史に戊子朔とある。したがって2月朔のユリウス暦日は2月20日となる。</t>
+    <rPh sb="29" eb="30">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天長 5年 3 小 丁巳  52-2600</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では52丙辰であるが，逸史によれば丁巳朔，閏3月丙戌朔であるから3月朔は丁巳以外にない。したがって3月朔のユリウス暦日は3月20日となる。</t>
+    <rPh sb="23" eb="24">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>イガイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天長 7年 6 小 甲辰 39-1519</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>逸史巻30，2月癸亥朔とある。したがって2月朔日のユリウス暦日は2月26日。</t>
+    <rPh sb="10" eb="11">
+      <t>サクジテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>逸史巻38，6月甲辰朔とある。計算は39癸卯，したがって6月朔のユリウス暦日は6月25日。</t>
+    <rPh sb="10" eb="11">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>2021/07/27</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天長 7年 7 小 癸酉 8-2856</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では8壬申であるが，癸酉にしなければ6月が28日になってしまう。したがって7月朔のユリウス暦日は7月24日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ジn</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では30甲午, 逸史により乙未，計算C）では乙未−25。したがって正月朔のユリウス暦日は2月6日。</t>
+    <rPh sb="10" eb="11">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t xml:space="preserve">ニホンキ </t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 2年 1 小 丁未 42-2793</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は42丙午，続日本後紀により丁未，したがって正月朔ユリウス暦日は2月2日となる。天長10年より嘉祥2年（西暦849年）までは続日本後紀に全月朔干支がでている。それによると，この頁の3年間で計算と干支の違うのはこの承和2年正月のみで，この年の4月，10月などは小余が大きくても進朔していないことがわかる。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ニホn</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>コウキ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t xml:space="preserve">キ </t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ニティ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>テn</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ナガイ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ネn</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>ネn</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>セイレキ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ネn</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ニホn</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ゼn</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t xml:space="preserve">サク </t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>カンセィ</t>
+    </rPh>
+    <rPh sb="90" eb="91">
+      <t xml:space="preserve">ページ </t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>ネn</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>カンセィ</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>チガ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="111" eb="112">
+      <t>ネn</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="120" eb="121">
+      <t>トセィ</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="127" eb="128">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="134" eb="135">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="139" eb="141">
+      <t>シンサク</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 3年 8 小 戊戌 33-2996</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は33丁酉，続後紀戊戌朔，したがって8月朔日のユリウス暦日は9月15日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>コウキ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>_x0002__x0004__x0008__x0001_</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>_x0006_	_x0001_</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">	
+_x0001__x000B__x000D_</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>_x0001__x000F__x0015_</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 3年 10 小 丁酉 32-3000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は32丙申，続後紀丁酉朔，したがって10月朔日のユリウス暦日は11月13日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>コウキ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>_x0002__x0004__x0008__x0001_</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>_x0006_	_x0001_</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">	
+_x0001__x000B__x000D_</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>_x0001__x000F__x0016_</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 5年 9 小 丙辰 51-2800</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は51乙卯，続後紀丙辰朔，したがって9月朔日のユリウス暦日は9月23日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ゾク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>コウキ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>_x0002__x0004__x0006__x0001_</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 6年 8 小 庚戌 45-2916</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は45己酉，続後紀は庚戌朔，したがって8月朔日のユリウス暦日は9月12日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>コウキ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>_x0002__x0004__x0005__x0001_</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 6年 12 小 己酉 44-2892</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は44戊申，続後紀は己酉朔，したがって12月朔日のユリウス暦日は1月9日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>コウキ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>_x0002__x0004__x0005__x0001_</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 9年 3 小 丙申 31-2738</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は31乙未，続後紀は丙申朔，したがって3月朔日のユリウス暦日は4月15日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>_x0002__x0004__x0007__x0001_</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 9年 12 小 辛酉 56-2661</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は56庚申，続後紀は辛酉朔，したがって12月朔日のユリウス暦日は1月5日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>_x0002__x0004__x0005__x0001_</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 11年 6 小 癸丑 48-2934</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は48壬子，続後紀は癸丑朔，したがって6月朔日のユリウス暦日は6月20日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>_x0002__x0004__x0005__x0001_</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 11年 9 小 辛亥 46-2695</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は46庚戌，続後紀は辛亥朔，したがって9月朔日のユリウス暦日は10月16日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 12年 10 小 乙亥 10-2799</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は10甲戌，続後紀は乙亥朔，したがって10月朔日のユリウス暦日は11月4日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 12年 12 小 甲戌 9-2726</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 13年 11 小 己亥  34-2812</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 14年 5 小 乙丑 0-2867</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承和 14年 11 小 癸亥 58-2640</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は9癸酉，続後紀は甲戌朔，したがって12月朔日のユリウス暦日は1月2日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は34戊戌，続後紀は己亥朔，したがって11月朔日のユリウス暦日は11月23日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は0甲子，続後紀は乙丑朔，したがって5月朔日のユリウス暦日は6月17日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は58壬戌，続後紀は癸亥朔，したがって11月朔日のユリウス暦日は12月12日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>嘉祥 1年 11 小 丁巳 52-2966</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は52丙辰，続後紀は丁巳朔，したがって11月朔日のユリウス暦日は11月30日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>嘉祥 2年 11 小 辛亥 46-2922</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は46庚戌，続後紀は辛亥朔，したがって11月朔日のユリウス暦日は11月19日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>嘉祥 3年 2 小 庚戌  45-2860</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は45己酉，続後紀は庚戌朔，したがって2月朔日のユリウス暦日は3月18日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>仁寿 3年 7 小 庚寅 25-2763</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は25己丑，文徳実録は庚寅朔，したがって7月朔日のユリウス暦日は8月9日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>_x0002__x0004_</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>斎衡 1年 12 大 壬子 47-2602</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では47辛亥であるが，文徳実録によれば，斎衡元年10月壬子朔，同2年正月壬午朔とあるから，12月朔は壬子でなければならない。したがってこの日のユリウス日は12月24日になる。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="13" eb="17">
+      <t>ブントク</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ガンネn</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>_x0000__x0000__x0002_</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>_x0004__x000D__x0004__x0008__x0018_</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>_x0002__x000C__x001C_</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>_x0001__x000F_</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>_x001F__x0001__x0014_!_x0001__x0017_</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>#_x0001__x0019_</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>$_x0002__x001F_</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>&amp;_x0002_"</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>(_x0001_%1_x0001_</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>(2</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>_x0001_-</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>G_x0001_/</t>
+    </rPh>
+    <rPh sb="84" eb="85">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では17辛巳，小余が小さく進朔とは思えない。文徳実録により壬午，したがって元日のユリウス暦日は1月23日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>チイサク</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>シンサ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>オモエ</t>
+    </rPh>
+    <rPh sb="22" eb="26">
+      <t>ブントク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ジn</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ガンジテゥ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>斎衡 2年 2 小 辛亥 46-2139</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算では46庚戌となるが，文徳実録に正月壬午朔，4月己酉朔とあるから2月朔は辛亥しかない。したがって2月朔のユリウス暦日は2月21日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="11" eb="15">
+      <t>ブントク</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジンゴ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>2021/07/27</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>斎衡 2年 12 小 丙子 11-2894</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>斎衡 3年 10 小 辛未 6-2919</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は11乙亥，文徳実録は丙子朔，したがって12月朔日のユリウス暦日は1月12日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>_x0002__x0004_</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は6庚午，文徳実録は辛未朔，したがって10月朔日のユリウス暦日は11月2日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイ_x0000__x0000_</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>_x0002__x0004_</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天安 1年 1 小 庚子 35-2985</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は35己亥，文徳実録は庚子朔，したがって正月朔日のユリウス暦日は1月30日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t/>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天安 1年 10 小 乙丑  0-2932</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は0甲子，文徳実録は乙丑朔，したがって10月朔日のユリウス暦日は10月22日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>天安 2年 2 小 甲子 59-2856</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は59癸亥，文徳実録は甲子朔，したがって2月朔日のユリウス暦日は2月18日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は18壬午，三代実録は癸未朔，したがって10月朔日のユリウス暦日は10月30日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>貞観 2年 2 小 壬午 17-2710</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は17辛巳，三代実録は壬午朔，したがって2月朔日のユリウス暦日は2月26日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>貞観 2年 閏10 大 丁未  42-2908</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は42丙午，三代実録は丁未朔，したがって閏10月朔日のユリウス暦日は11月17日。この進朔によって中気を含まない月がずれ閏が9月から10月に変る。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>シンサ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>フクマナ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>ツキ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ウルウ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>カワ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は12丙子，しかし冬至が13丁丑であるから朔旦冬至にするため丁丑にかえた。したがって11月朔日のユリウス暦日は12月17日である。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサn</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>トウジ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ガンタn</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>トウジ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>サクジテゥ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ガテゥ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ニティ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は11乙亥，三代実録は丙子朔，したがって正月朔日のユリウス暦日は2月14日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>貞観 3年 4 小 乙巳 40-2910</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>貞観 3年 6 小 甲辰 39-2990</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は40甲辰，三代実録は乙巳朔，したがって4月朔日のユリウス暦日は5月14日，五紀暦では41（乙巳）ー14とでる。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t xml:space="preserve">イツツ </t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t xml:space="preserve">キ </t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>レキ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>計算は39癸卯，三代実録は甲辰朔，したがって6月朔日のユリウス暦日は7月12日。</t>
+    <rPh sb="0" eb="2">
+      <t>ケイショ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ショウガテゥ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ショウガテゥ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -6669,7 +7952,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -6691,6 +7974,19 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="ヒラギノ角ゴ ProN W3"/>
       <family val="2"/>
       <charset val="128"/>
@@ -7022,7 +8318,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -7189,6 +8485,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8350,11 +9658,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG447"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="211" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H91" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H241" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I104" sqref="I104"/>
+      <selection pane="bottomRight" activeCell="I247" sqref="I247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="20" customHeight="1"/>
@@ -8681,7 +9989,7 @@
         <v>1429</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>1639</v>
+        <v>1585</v>
       </c>
       <c r="J5" s="33"/>
       <c r="K5" s="35" t="s">
@@ -8856,10 +10164,10 @@
         <v>1190</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>1640</v>
+        <v>1586</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>1641</v>
+        <v>1587</v>
       </c>
       <c r="J8" s="33"/>
       <c r="K8" s="35" t="s">
@@ -9092,10 +10400,10 @@
         <v>1194</v>
       </c>
       <c r="H12" s="49" t="s">
-        <v>1642</v>
+        <v>1588</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>1644</v>
+        <v>1590</v>
       </c>
       <c r="J12" s="46"/>
       <c r="K12" s="35" t="s">
@@ -9137,7 +10445,7 @@
         <v>956</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>1645</v>
+        <v>1591</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>957</v>
@@ -9152,7 +10460,7 @@
         <v>1195</v>
       </c>
       <c r="H13" s="50" t="s">
-        <v>1647</v>
+        <v>1593</v>
       </c>
       <c r="I13" s="35" t="s">
         <v>912</v>
@@ -9197,7 +10505,7 @@
         <v>957</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>1645</v>
+        <v>1591</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>912</v>
@@ -9212,10 +10520,10 @@
         <v>1196</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>1648</v>
+        <v>1594</v>
       </c>
       <c r="I14" s="35" t="s">
-        <v>1649</v>
+        <v>1595</v>
       </c>
       <c r="J14" s="33"/>
       <c r="K14" s="35" t="s">
@@ -9254,7 +10562,7 @@
     </row>
     <row r="15" spans="2:33" s="20" customFormat="1" ht="48.5" customHeight="1">
       <c r="B15" s="29" t="s">
-        <v>1645</v>
+        <v>1591</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>912</v>
@@ -9275,7 +10583,7 @@
         <v>912</v>
       </c>
       <c r="I15" s="35" t="s">
-        <v>1646</v>
+        <v>1592</v>
       </c>
       <c r="J15" s="33"/>
       <c r="K15" s="52" t="s">
@@ -9964,10 +11272,10 @@
         <v>1208</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>1650</v>
+        <v>1596</v>
       </c>
       <c r="I27" s="35" t="s">
-        <v>1651</v>
+        <v>1597</v>
       </c>
       <c r="J27" s="33"/>
       <c r="K27" s="35" t="s">
@@ -10084,10 +11392,10 @@
         <v>1210</v>
       </c>
       <c r="H29" s="50" t="s">
-        <v>1652</v>
+        <v>1598</v>
       </c>
       <c r="I29" s="35" t="s">
-        <v>1653</v>
+        <v>1599</v>
       </c>
       <c r="J29" s="33"/>
       <c r="K29" s="35" t="s">
@@ -10204,10 +11512,10 @@
         <v>1212</v>
       </c>
       <c r="H31" s="50" t="s">
-        <v>1654</v>
+        <v>1600</v>
       </c>
       <c r="I31" s="35" t="s">
-        <v>1655</v>
+        <v>1601</v>
       </c>
       <c r="J31" s="33"/>
       <c r="K31" s="35" t="s">
@@ -10324,10 +11632,10 @@
         <v>1214</v>
       </c>
       <c r="H33" s="50" t="s">
-        <v>1656</v>
+        <v>1602</v>
       </c>
       <c r="I33" s="35" t="s">
-        <v>1658</v>
+        <v>1604</v>
       </c>
       <c r="J33" s="33"/>
       <c r="K33" s="35" t="s">
@@ -10384,7 +11692,7 @@
         <v>1215</v>
       </c>
       <c r="H34" s="50" t="s">
-        <v>1657</v>
+        <v>1603</v>
       </c>
       <c r="I34" s="35" t="s">
         <v>912</v>
@@ -10500,10 +11808,10 @@
         <v>1217</v>
       </c>
       <c r="H36" s="50" t="s">
-        <v>1659</v>
+        <v>1605</v>
       </c>
       <c r="I36" s="35" t="s">
-        <v>1660</v>
+        <v>1606</v>
       </c>
       <c r="J36" s="33"/>
       <c r="K36" s="35" t="s">
@@ -10567,7 +11875,7 @@
         <v>1450</v>
       </c>
       <c r="I37" s="35" t="s">
-        <v>1661</v>
+        <v>1607</v>
       </c>
       <c r="J37" s="33"/>
       <c r="K37" s="35" t="s">
@@ -10628,10 +11936,10 @@
         <v>1218</v>
       </c>
       <c r="H38" s="50" t="s">
-        <v>1662</v>
+        <v>1608</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>1663</v>
+        <v>1609</v>
       </c>
       <c r="J38" s="35" t="s">
         <v>932</v>
@@ -10746,10 +12054,10 @@
         <v>1220</v>
       </c>
       <c r="H40" s="50" t="s">
-        <v>1664</v>
+        <v>1610</v>
       </c>
       <c r="I40" s="35" t="s">
-        <v>1665</v>
+        <v>1611</v>
       </c>
       <c r="J40" s="33"/>
       <c r="K40" s="35" t="s">
@@ -10809,7 +12117,7 @@
         <v>1452</v>
       </c>
       <c r="I41" s="35" t="s">
-        <v>1666</v>
+        <v>1612</v>
       </c>
       <c r="J41" s="33"/>
       <c r="K41" s="35" t="s">
@@ -10870,10 +12178,10 @@
         <v>1222</v>
       </c>
       <c r="H42" s="50" t="s">
-        <v>1667</v>
+        <v>1613</v>
       </c>
       <c r="I42" s="35" t="s">
-        <v>1668</v>
+        <v>1614</v>
       </c>
       <c r="J42" s="33"/>
       <c r="K42" s="35" t="s">
@@ -11168,10 +12476,10 @@
         <v>1227</v>
       </c>
       <c r="H47" s="50" t="s">
-        <v>1669</v>
+        <v>1615</v>
       </c>
       <c r="I47" s="35" t="s">
-        <v>1670</v>
+        <v>1616</v>
       </c>
       <c r="J47" s="35"/>
       <c r="K47" s="35" t="s">
@@ -11346,10 +12654,10 @@
         <v>1230</v>
       </c>
       <c r="H50" s="50" t="s">
-        <v>1671</v>
+        <v>1617</v>
       </c>
       <c r="I50" s="35" t="s">
-        <v>1672</v>
+        <v>1618</v>
       </c>
       <c r="J50" s="35"/>
       <c r="K50" s="35" t="s">
@@ -11466,10 +12774,10 @@
         <v>1232</v>
       </c>
       <c r="H52" s="50" t="s">
-        <v>1674</v>
+        <v>1620</v>
       </c>
       <c r="I52" s="35" t="s">
-        <v>1675</v>
+        <v>1621</v>
       </c>
       <c r="J52" s="35"/>
       <c r="K52" s="35" t="s">
@@ -11644,10 +12952,10 @@
         <v>1235</v>
       </c>
       <c r="H55" s="50" t="s">
-        <v>1676</v>
+        <v>1622</v>
       </c>
       <c r="I55" s="35" t="s">
-        <v>1677</v>
+        <v>1623</v>
       </c>
       <c r="J55" s="35"/>
       <c r="K55" s="35" t="s">
@@ -11704,7 +13012,7 @@
         <v>1236</v>
       </c>
       <c r="H56" s="50" t="s">
-        <v>1678</v>
+        <v>1624</v>
       </c>
       <c r="I56" s="35" t="s">
         <v>912</v>
@@ -11767,7 +13075,7 @@
         <v>1462</v>
       </c>
       <c r="I57" s="35" t="s">
-        <v>1679</v>
+        <v>1625</v>
       </c>
       <c r="J57" s="35"/>
       <c r="K57" s="35" t="s">
@@ -11888,10 +13196,10 @@
         <v>1239</v>
       </c>
       <c r="H59" s="50" t="s">
-        <v>1680</v>
+        <v>1626</v>
       </c>
       <c r="I59" s="35" t="s">
-        <v>1681</v>
+        <v>1627</v>
       </c>
       <c r="J59" s="35"/>
       <c r="K59" s="35" t="s">
@@ -12012,10 +13320,10 @@
         <v>1241</v>
       </c>
       <c r="H61" s="50" t="s">
-        <v>1682</v>
+        <v>1628</v>
       </c>
       <c r="I61" s="35" t="s">
-        <v>1683</v>
+        <v>1629</v>
       </c>
       <c r="J61" s="35"/>
       <c r="K61" s="35" t="s">
@@ -12132,10 +13440,10 @@
         <v>1243</v>
       </c>
       <c r="H63" s="50" t="s">
-        <v>1684</v>
+        <v>1630</v>
       </c>
       <c r="I63" s="35" t="s">
-        <v>1685</v>
+        <v>1631</v>
       </c>
       <c r="J63" s="35"/>
       <c r="K63" s="35" t="s">
@@ -12368,10 +13676,10 @@
         <v>1247</v>
       </c>
       <c r="H67" s="50" t="s">
-        <v>1686</v>
+        <v>1632</v>
       </c>
       <c r="I67" s="35" t="s">
-        <v>1690</v>
+        <v>1636</v>
       </c>
       <c r="J67" s="35"/>
       <c r="K67" s="35" t="s">
@@ -12428,7 +13736,7 @@
         <v>1248</v>
       </c>
       <c r="H68" s="50" t="s">
-        <v>1687</v>
+        <v>1633</v>
       </c>
       <c r="I68" s="35" t="s">
         <v>912</v>
@@ -12488,7 +13796,7 @@
         <v>1249</v>
       </c>
       <c r="H69" s="50" t="s">
-        <v>1688</v>
+        <v>1634</v>
       </c>
       <c r="I69" s="35" t="s">
         <v>912</v>
@@ -12548,7 +13856,7 @@
         <v>1250</v>
       </c>
       <c r="H70" s="50" t="s">
-        <v>1689</v>
+        <v>1635</v>
       </c>
       <c r="I70" s="35" t="s">
         <v>912</v>
@@ -12668,10 +13976,10 @@
         <v>1252</v>
       </c>
       <c r="H72" s="50" t="s">
-        <v>1691</v>
+        <v>1637</v>
       </c>
       <c r="I72" s="35" t="s">
-        <v>1692</v>
+        <v>1638</v>
       </c>
       <c r="J72" s="33"/>
       <c r="K72" s="35" t="s">
@@ -12728,7 +14036,7 @@
         <v>1253</v>
       </c>
       <c r="H73" s="50" t="s">
-        <v>1693</v>
+        <v>1639</v>
       </c>
       <c r="I73" s="55" t="s">
         <v>912</v>
@@ -12791,7 +14099,7 @@
         <v>1470</v>
       </c>
       <c r="I74" s="35" t="s">
-        <v>1694</v>
+        <v>1640</v>
       </c>
       <c r="J74" s="33"/>
       <c r="K74" s="35" t="s">
@@ -12851,7 +14159,7 @@
         <v>1471</v>
       </c>
       <c r="I75" s="35" t="s">
-        <v>1695</v>
+        <v>1641</v>
       </c>
       <c r="J75" s="33"/>
       <c r="K75" s="35" t="s">
@@ -12971,10 +14279,10 @@
         <v>1473</v>
       </c>
       <c r="I77" s="35" t="s">
-        <v>1698</v>
+        <v>1644</v>
       </c>
       <c r="J77" s="35" t="s">
-        <v>1697</v>
+        <v>1643</v>
       </c>
       <c r="K77" s="35" t="s">
         <v>942</v>
@@ -13090,10 +14398,10 @@
         <v>1259</v>
       </c>
       <c r="H79" s="50" t="s">
-        <v>1699</v>
+        <v>1645</v>
       </c>
       <c r="I79" s="35" t="s">
-        <v>1700</v>
+        <v>1646</v>
       </c>
       <c r="J79" s="33"/>
       <c r="K79" s="35" t="s">
@@ -13153,7 +14461,7 @@
         <v>1475</v>
       </c>
       <c r="I80" s="35" t="s">
-        <v>1701</v>
+        <v>1647</v>
       </c>
       <c r="J80" s="33"/>
       <c r="K80" s="35" t="s">
@@ -13213,7 +14521,7 @@
         <v>1476</v>
       </c>
       <c r="I81" s="35" t="s">
-        <v>1702</v>
+        <v>1648</v>
       </c>
       <c r="J81" s="35" t="s">
         <v>934</v>
@@ -13331,7 +14639,7 @@
         <v>1478</v>
       </c>
       <c r="I83" s="35" t="s">
-        <v>1703</v>
+        <v>1649</v>
       </c>
       <c r="J83" s="33"/>
       <c r="K83" s="35" t="s">
@@ -13451,7 +14759,7 @@
         <v>1480</v>
       </c>
       <c r="I85" s="35" t="s">
-        <v>1704</v>
+        <v>1650</v>
       </c>
       <c r="J85" s="33"/>
       <c r="K85" s="35" t="s">
@@ -13571,7 +14879,7 @@
         <v>1482</v>
       </c>
       <c r="I87" s="35" t="s">
-        <v>1705</v>
+        <v>1651</v>
       </c>
       <c r="J87" s="33"/>
       <c r="K87" s="35" t="s">
@@ -13804,10 +15112,10 @@
         <v>1271</v>
       </c>
       <c r="H91" s="50" t="s">
-        <v>1706</v>
+        <v>1652</v>
       </c>
       <c r="I91" s="35" t="s">
-        <v>1708</v>
+        <v>1654</v>
       </c>
       <c r="J91" s="35"/>
       <c r="K91" s="35" t="s">
@@ -13927,7 +15235,7 @@
         <v>1487</v>
       </c>
       <c r="I93" s="35" t="s">
-        <v>1709</v>
+        <v>1655</v>
       </c>
       <c r="J93" s="35"/>
       <c r="K93" s="35" t="s">
@@ -14047,7 +15355,7 @@
         <v>1489</v>
       </c>
       <c r="I95" s="35" t="s">
-        <v>1710</v>
+        <v>1656</v>
       </c>
       <c r="J95" s="35"/>
       <c r="K95" s="35" t="s">
@@ -14222,10 +15530,10 @@
         <v>1278</v>
       </c>
       <c r="H98" s="50" t="s">
-        <v>1707</v>
+        <v>1653</v>
       </c>
       <c r="I98" s="35" t="s">
-        <v>1711</v>
+        <v>1657</v>
       </c>
       <c r="J98" s="35"/>
       <c r="K98" s="35" t="s">
@@ -14458,10 +15766,10 @@
         <v>1282</v>
       </c>
       <c r="H102" s="50" t="s">
-        <v>1712</v>
+        <v>1658</v>
       </c>
       <c r="I102" s="35" t="s">
-        <v>1713</v>
+        <v>1659</v>
       </c>
       <c r="J102" s="35"/>
       <c r="K102" s="35" t="s">
@@ -14580,7 +15888,9 @@
       <c r="H104" s="50" t="s">
         <v>1496</v>
       </c>
-      <c r="I104" s="35"/>
+      <c r="I104" s="35" t="s">
+        <v>1660</v>
+      </c>
       <c r="J104" s="35"/>
       <c r="K104" s="35" t="s">
         <v>942</v>
@@ -14638,7 +15948,9 @@
       <c r="H105" s="50" t="s">
         <v>1497</v>
       </c>
-      <c r="I105" s="35"/>
+      <c r="I105" s="55" t="s">
+        <v>912</v>
+      </c>
       <c r="J105" s="35"/>
       <c r="K105" s="35" t="s">
         <v>942</v>
@@ -14694,9 +16006,11 @@
         <v>1286</v>
       </c>
       <c r="H106" s="50" t="s">
-        <v>1498</v>
-      </c>
-      <c r="I106" s="35"/>
+        <v>1661</v>
+      </c>
+      <c r="I106" s="35" t="s">
+        <v>1662</v>
+      </c>
       <c r="J106" s="35"/>
       <c r="K106" s="35" t="s">
         <v>942</v>
@@ -14752,9 +16066,11 @@
         <v>1287</v>
       </c>
       <c r="H107" s="50" t="s">
-        <v>1499</v>
-      </c>
-      <c r="I107" s="35"/>
+        <v>1498</v>
+      </c>
+      <c r="I107" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J107" s="35"/>
       <c r="K107" s="35" t="s">
         <v>942</v>
@@ -14810,9 +16126,11 @@
         <v>1288</v>
       </c>
       <c r="H108" s="50" t="s">
-        <v>1500</v>
-      </c>
-      <c r="I108" s="35"/>
+        <v>1663</v>
+      </c>
+      <c r="I108" s="35" t="s">
+        <v>1664</v>
+      </c>
       <c r="J108" s="35"/>
       <c r="K108" s="35" t="s">
         <v>942</v>
@@ -14868,9 +16186,11 @@
         <v>1289</v>
       </c>
       <c r="H109" s="50" t="s">
-        <v>1501</v>
-      </c>
-      <c r="I109" s="35"/>
+        <v>1499</v>
+      </c>
+      <c r="I109" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J109" s="35"/>
       <c r="K109" s="35" t="s">
         <v>942</v>
@@ -14926,9 +16246,11 @@
         <v>1290</v>
       </c>
       <c r="H110" s="50" t="s">
-        <v>1502</v>
-      </c>
-      <c r="I110" s="35"/>
+        <v>1500</v>
+      </c>
+      <c r="I110" s="35" t="s">
+        <v>1665</v>
+      </c>
       <c r="J110" s="35"/>
       <c r="K110" s="35" t="s">
         <v>942</v>
@@ -14984,9 +16306,11 @@
         <v>1291</v>
       </c>
       <c r="H111" s="50" t="s">
-        <v>1503</v>
-      </c>
-      <c r="I111" s="35"/>
+        <v>1501</v>
+      </c>
+      <c r="I111" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J111" s="35" t="s">
         <v>934</v>
       </c>
@@ -15040,9 +16364,11 @@
         <v>1292</v>
       </c>
       <c r="H112" s="50" t="s">
-        <v>1504</v>
-      </c>
-      <c r="I112" s="35"/>
+        <v>1502</v>
+      </c>
+      <c r="I112" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J112" s="35" t="s">
         <v>934</v>
       </c>
@@ -15096,9 +16422,11 @@
         <v>1293</v>
       </c>
       <c r="H113" s="50" t="s">
-        <v>1505</v>
-      </c>
-      <c r="I113" s="35"/>
+        <v>1503</v>
+      </c>
+      <c r="I113" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J113" s="35" t="s">
         <v>934</v>
       </c>
@@ -15152,9 +16480,11 @@
         <v>1294</v>
       </c>
       <c r="H114" s="50" t="s">
-        <v>1506</v>
-      </c>
-      <c r="I114" s="35"/>
+        <v>1504</v>
+      </c>
+      <c r="I114" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J114" s="35"/>
       <c r="K114" s="35" t="s">
         <v>942</v>
@@ -15210,9 +16540,11 @@
         <v>1295</v>
       </c>
       <c r="H115" s="50" t="s">
-        <v>1507</v>
-      </c>
-      <c r="I115" s="35"/>
+        <v>1666</v>
+      </c>
+      <c r="I115" s="35" t="s">
+        <v>1667</v>
+      </c>
       <c r="J115" s="35"/>
       <c r="K115" s="35" t="s">
         <v>942</v>
@@ -15268,9 +16600,11 @@
         <v>1296</v>
       </c>
       <c r="H116" s="50" t="s">
-        <v>1508</v>
-      </c>
-      <c r="I116" s="35"/>
+        <v>1505</v>
+      </c>
+      <c r="I116" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J116" s="35"/>
       <c r="K116" s="35" t="s">
         <v>942</v>
@@ -15326,9 +16660,11 @@
         <v>1297</v>
       </c>
       <c r="H117" s="50" t="s">
-        <v>1509</v>
-      </c>
-      <c r="I117" s="35"/>
+        <v>1506</v>
+      </c>
+      <c r="I117" s="35" t="s">
+        <v>1668</v>
+      </c>
       <c r="J117" s="35"/>
       <c r="K117" s="35" t="s">
         <v>942</v>
@@ -15384,9 +16720,11 @@
         <v>1298</v>
       </c>
       <c r="H118" s="50" t="s">
-        <v>1510</v>
-      </c>
-      <c r="I118" s="35"/>
+        <v>1507</v>
+      </c>
+      <c r="I118" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J118" s="35"/>
       <c r="K118" s="35" t="s">
         <v>942</v>
@@ -15442,9 +16780,11 @@
         <v>1299</v>
       </c>
       <c r="H119" s="50" t="s">
-        <v>1511</v>
-      </c>
-      <c r="I119" s="35"/>
+        <v>1669</v>
+      </c>
+      <c r="I119" s="35" t="s">
+        <v>1670</v>
+      </c>
       <c r="J119" s="35"/>
       <c r="K119" s="35" t="s">
         <v>942</v>
@@ -15500,9 +16840,11 @@
         <v>1300</v>
       </c>
       <c r="H120" s="50" t="s">
-        <v>1512</v>
-      </c>
-      <c r="I120" s="35"/>
+        <v>1508</v>
+      </c>
+      <c r="I120" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J120" s="35"/>
       <c r="K120" s="35" t="s">
         <v>942</v>
@@ -15558,9 +16900,11 @@
         <v>1301</v>
       </c>
       <c r="H121" s="50" t="s">
-        <v>1513</v>
-      </c>
-      <c r="I121" s="35"/>
+        <v>1671</v>
+      </c>
+      <c r="I121" s="35" t="s">
+        <v>1672</v>
+      </c>
       <c r="J121" s="35"/>
       <c r="K121" s="35" t="s">
         <v>942</v>
@@ -15616,9 +16960,11 @@
         <v>1302</v>
       </c>
       <c r="H122" s="50" t="s">
-        <v>1514</v>
-      </c>
-      <c r="I122" s="35"/>
+        <v>1509</v>
+      </c>
+      <c r="I122" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J122" s="35" t="s">
         <v>934</v>
       </c>
@@ -15672,9 +17018,11 @@
         <v>1303</v>
       </c>
       <c r="H123" s="50" t="s">
-        <v>1515</v>
-      </c>
-      <c r="I123" s="35"/>
+        <v>1510</v>
+      </c>
+      <c r="I123" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J123" s="35"/>
       <c r="K123" s="35" t="s">
         <v>942</v>
@@ -15730,9 +17078,11 @@
         <v>1304</v>
       </c>
       <c r="H124" s="50" t="s">
-        <v>1516</v>
-      </c>
-      <c r="I124" s="35"/>
+        <v>1673</v>
+      </c>
+      <c r="I124" s="35" t="s">
+        <v>1674</v>
+      </c>
       <c r="J124" s="35"/>
       <c r="K124" s="35" t="s">
         <v>942</v>
@@ -15788,9 +17138,11 @@
         <v>1305</v>
       </c>
       <c r="H125" s="50" t="s">
-        <v>1517</v>
-      </c>
-      <c r="I125" s="35"/>
+        <v>1511</v>
+      </c>
+      <c r="I125" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J125" s="35"/>
       <c r="K125" s="35" t="s">
         <v>942</v>
@@ -15846,9 +17198,11 @@
         <v>1306</v>
       </c>
       <c r="H126" s="50" t="s">
-        <v>1518</v>
-      </c>
-      <c r="I126" s="35"/>
+        <v>1675</v>
+      </c>
+      <c r="I126" s="35" t="s">
+        <v>1676</v>
+      </c>
       <c r="J126" s="35"/>
       <c r="K126" s="35" t="s">
         <v>942</v>
@@ -15904,9 +17258,11 @@
         <v>1307</v>
       </c>
       <c r="H127" s="50" t="s">
-        <v>1519</v>
-      </c>
-      <c r="I127" s="35"/>
+        <v>1512</v>
+      </c>
+      <c r="I127" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J127" s="35" t="s">
         <v>934</v>
       </c>
@@ -15960,9 +17316,11 @@
         <v>1308</v>
       </c>
       <c r="H128" s="50" t="s">
-        <v>1520</v>
-      </c>
-      <c r="I128" s="35"/>
+        <v>1513</v>
+      </c>
+      <c r="I128" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J128" s="35" t="s">
         <v>934</v>
       </c>
@@ -16016,9 +17374,11 @@
         <v>1309</v>
       </c>
       <c r="H129" s="50" t="s">
-        <v>1521</v>
-      </c>
-      <c r="I129" s="35"/>
+        <v>1514</v>
+      </c>
+      <c r="I129" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J129" s="35" t="s">
         <v>934</v>
       </c>
@@ -16072,9 +17432,11 @@
         <v>1310</v>
       </c>
       <c r="H130" s="50" t="s">
-        <v>1522</v>
-      </c>
-      <c r="I130" s="35"/>
+        <v>1515</v>
+      </c>
+      <c r="I130" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J130" s="35"/>
       <c r="K130" s="35" t="s">
         <v>942</v>
@@ -16130,9 +17492,11 @@
         <v>1311</v>
       </c>
       <c r="H131" s="50" t="s">
-        <v>1523</v>
-      </c>
-      <c r="I131" s="35"/>
+        <v>1677</v>
+      </c>
+      <c r="I131" s="35" t="s">
+        <v>1678</v>
+      </c>
       <c r="J131" s="35"/>
       <c r="K131" s="35" t="s">
         <v>942</v>
@@ -16188,9 +17552,11 @@
         <v>1312</v>
       </c>
       <c r="H132" s="50" t="s">
-        <v>1524</v>
-      </c>
-      <c r="I132" s="35"/>
+        <v>1516</v>
+      </c>
+      <c r="I132" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J132" s="35" t="s">
         <v>934</v>
       </c>
@@ -16244,9 +17610,11 @@
         <v>1313</v>
       </c>
       <c r="H133" s="50" t="s">
-        <v>1525</v>
-      </c>
-      <c r="I133" s="35"/>
+        <v>1517</v>
+      </c>
+      <c r="I133" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J133" s="35"/>
       <c r="K133" s="35" t="s">
         <v>942</v>
@@ -16302,9 +17670,11 @@
         <v>1314</v>
       </c>
       <c r="H134" s="50" t="s">
-        <v>1526</v>
-      </c>
-      <c r="I134" s="35"/>
+        <v>1679</v>
+      </c>
+      <c r="I134" s="35" t="s">
+        <v>1680</v>
+      </c>
       <c r="J134" s="35"/>
       <c r="K134" s="35" t="s">
         <v>942</v>
@@ -16360,9 +17730,11 @@
         <v>1315</v>
       </c>
       <c r="H135" s="50" t="s">
-        <v>1527</v>
-      </c>
-      <c r="I135" s="35"/>
+        <v>1518</v>
+      </c>
+      <c r="I135" s="35" t="s">
+        <v>1681</v>
+      </c>
       <c r="J135" s="35"/>
       <c r="K135" s="35" t="s">
         <v>942</v>
@@ -16418,9 +17790,11 @@
         <v>1316</v>
       </c>
       <c r="H136" s="50" t="s">
-        <v>1528</v>
-      </c>
-      <c r="I136" s="35"/>
+        <v>1519</v>
+      </c>
+      <c r="I136" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J136" s="35"/>
       <c r="K136" s="35" t="s">
         <v>942</v>
@@ -16476,9 +17850,11 @@
         <v>1317</v>
       </c>
       <c r="H137" s="50" t="s">
-        <v>1529</v>
-      </c>
-      <c r="I137" s="35"/>
+        <v>1682</v>
+      </c>
+      <c r="I137" s="35" t="s">
+        <v>1683</v>
+      </c>
       <c r="J137" s="35"/>
       <c r="K137" s="35" t="s">
         <v>942</v>
@@ -16534,9 +17910,11 @@
         <v>1318</v>
       </c>
       <c r="H138" s="50" t="s">
-        <v>1530</v>
-      </c>
-      <c r="I138" s="35"/>
+        <v>1520</v>
+      </c>
+      <c r="I138" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J138" s="35" t="s">
         <v>934</v>
       </c>
@@ -16590,9 +17968,11 @@
         <v>1319</v>
       </c>
       <c r="H139" s="50" t="s">
-        <v>1531</v>
-      </c>
-      <c r="I139" s="35"/>
+        <v>1521</v>
+      </c>
+      <c r="I139" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J139" s="35"/>
       <c r="K139" s="35" t="s">
         <v>942</v>
@@ -16648,9 +18028,11 @@
         <v>1320</v>
       </c>
       <c r="H140" s="50" t="s">
-        <v>1532</v>
-      </c>
-      <c r="I140" s="35"/>
+        <v>1684</v>
+      </c>
+      <c r="I140" s="35" t="s">
+        <v>1685</v>
+      </c>
       <c r="J140" s="35"/>
       <c r="K140" s="35" t="s">
         <v>942</v>
@@ -16706,9 +18088,11 @@
         <v>1321</v>
       </c>
       <c r="H141" s="50" t="s">
-        <v>1533</v>
-      </c>
-      <c r="I141" s="35"/>
+        <v>1522</v>
+      </c>
+      <c r="I141" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J141" s="35" t="s">
         <v>934</v>
       </c>
@@ -16762,9 +18146,11 @@
         <v>1322</v>
       </c>
       <c r="H142" s="50" t="s">
-        <v>1534</v>
-      </c>
-      <c r="I142" s="35"/>
+        <v>1523</v>
+      </c>
+      <c r="I142" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J142" s="35"/>
       <c r="K142" s="35" t="s">
         <v>942</v>
@@ -16820,9 +18206,11 @@
         <v>1323</v>
       </c>
       <c r="H143" s="50" t="s">
-        <v>1535</v>
-      </c>
-      <c r="I143" s="35"/>
+        <v>1686</v>
+      </c>
+      <c r="I143" s="35" t="s">
+        <v>1687</v>
+      </c>
       <c r="J143" s="35"/>
       <c r="K143" s="35" t="s">
         <v>942</v>
@@ -16878,9 +18266,11 @@
         <v>1324</v>
       </c>
       <c r="H144" s="50" t="s">
-        <v>1536</v>
-      </c>
-      <c r="I144" s="35"/>
+        <v>1524</v>
+      </c>
+      <c r="I144" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J144" s="35" t="s">
         <v>934</v>
       </c>
@@ -16934,9 +18324,11 @@
         <v>1325</v>
       </c>
       <c r="H145" s="50" t="s">
-        <v>1537</v>
-      </c>
-      <c r="I145" s="35"/>
+        <v>1525</v>
+      </c>
+      <c r="I145" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J145" s="35"/>
       <c r="K145" s="35" t="s">
         <v>942</v>
@@ -16992,9 +18384,11 @@
         <v>1326</v>
       </c>
       <c r="H146" s="50" t="s">
-        <v>1538</v>
-      </c>
-      <c r="I146" s="35"/>
+        <v>1688</v>
+      </c>
+      <c r="I146" s="35" t="s">
+        <v>1689</v>
+      </c>
       <c r="J146" s="35"/>
       <c r="K146" s="35" t="s">
         <v>942</v>
@@ -17050,9 +18444,11 @@
         <v>1327</v>
       </c>
       <c r="H147" s="50" t="s">
-        <v>1539</v>
-      </c>
-      <c r="I147" s="35"/>
+        <v>1526</v>
+      </c>
+      <c r="I147" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J147" s="35" t="s">
         <v>934</v>
       </c>
@@ -17106,9 +18502,11 @@
         <v>1328</v>
       </c>
       <c r="H148" s="50" t="s">
-        <v>1540</v>
-      </c>
-      <c r="I148" s="35"/>
+        <v>1527</v>
+      </c>
+      <c r="I148" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J148" s="35" t="s">
         <v>934</v>
       </c>
@@ -17162,9 +18560,11 @@
         <v>1329</v>
       </c>
       <c r="H149" s="50" t="s">
-        <v>1541</v>
-      </c>
-      <c r="I149" s="35"/>
+        <v>1528</v>
+      </c>
+      <c r="I149" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J149" s="35"/>
       <c r="K149" s="35" t="s">
         <v>942</v>
@@ -17220,9 +18620,11 @@
         <v>1330</v>
       </c>
       <c r="H150" s="50" t="s">
-        <v>1542</v>
-      </c>
-      <c r="I150" s="35"/>
+        <v>1690</v>
+      </c>
+      <c r="I150" s="35" t="s">
+        <v>1691</v>
+      </c>
       <c r="J150" s="35"/>
       <c r="K150" s="35" t="s">
         <v>942</v>
@@ -17278,9 +18680,11 @@
         <v>1331</v>
       </c>
       <c r="H151" s="50" t="s">
-        <v>1543</v>
-      </c>
-      <c r="I151" s="35"/>
+        <v>1529</v>
+      </c>
+      <c r="I151" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J151" s="35"/>
       <c r="K151" s="35" t="s">
         <v>942</v>
@@ -17336,9 +18740,11 @@
         <v>1332</v>
       </c>
       <c r="H152" s="50" t="s">
-        <v>1544</v>
-      </c>
-      <c r="I152" s="35"/>
+        <v>1692</v>
+      </c>
+      <c r="I152" s="35" t="s">
+        <v>1694</v>
+      </c>
       <c r="J152" s="35"/>
       <c r="K152" s="35" t="s">
         <v>942</v>
@@ -17394,9 +18800,11 @@
         <v>1333</v>
       </c>
       <c r="H153" s="50" t="s">
-        <v>1545</v>
-      </c>
-      <c r="I153" s="35"/>
+        <v>1530</v>
+      </c>
+      <c r="I153" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J153" s="35"/>
       <c r="K153" s="35" t="s">
         <v>942</v>
@@ -17452,9 +18860,11 @@
         <v>1334</v>
       </c>
       <c r="H154" s="50" t="s">
-        <v>1546</v>
-      </c>
-      <c r="I154" s="35"/>
+        <v>1693</v>
+      </c>
+      <c r="I154" s="35" t="s">
+        <v>1695</v>
+      </c>
       <c r="J154" s="35"/>
       <c r="K154" s="35" t="s">
         <v>942</v>
@@ -17510,9 +18920,11 @@
         <v>1335</v>
       </c>
       <c r="H155" s="50" t="s">
-        <v>1547</v>
-      </c>
-      <c r="I155" s="35"/>
+        <v>1696</v>
+      </c>
+      <c r="I155" s="35" t="s">
+        <v>1697</v>
+      </c>
       <c r="J155" s="35"/>
       <c r="K155" s="35" t="s">
         <v>942</v>
@@ -17568,9 +18980,11 @@
         <v>1336</v>
       </c>
       <c r="H156" s="50" t="s">
-        <v>1548</v>
-      </c>
-      <c r="I156" s="35"/>
+        <v>1531</v>
+      </c>
+      <c r="I156" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J156" s="35"/>
       <c r="K156" s="35" t="s">
         <v>942</v>
@@ -17626,9 +19040,11 @@
         <v>1337</v>
       </c>
       <c r="H157" s="50" t="s">
-        <v>1549</v>
-      </c>
-      <c r="I157" s="35"/>
+        <v>1698</v>
+      </c>
+      <c r="I157" s="35" t="s">
+        <v>1699</v>
+      </c>
       <c r="J157" s="35"/>
       <c r="K157" s="35" t="s">
         <v>942</v>
@@ -17684,9 +19100,11 @@
         <v>1338</v>
       </c>
       <c r="H158" s="50" t="s">
-        <v>1550</v>
-      </c>
-      <c r="I158" s="35"/>
+        <v>1532</v>
+      </c>
+      <c r="I158" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J158" s="35"/>
       <c r="K158" s="35" t="s">
         <v>942</v>
@@ -17742,9 +19160,11 @@
         <v>1339</v>
       </c>
       <c r="H159" s="50" t="s">
-        <v>1551</v>
-      </c>
-      <c r="I159" s="35"/>
+        <v>1533</v>
+      </c>
+      <c r="I159" s="35" t="s">
+        <v>1700</v>
+      </c>
       <c r="J159" s="35"/>
       <c r="K159" s="35" t="s">
         <v>942</v>
@@ -17800,9 +19220,11 @@
         <v>1340</v>
       </c>
       <c r="H160" s="50" t="s">
-        <v>1552</v>
-      </c>
-      <c r="I160" s="35"/>
+        <v>1534</v>
+      </c>
+      <c r="I160" s="35" t="s">
+        <v>1701</v>
+      </c>
       <c r="J160" s="35"/>
       <c r="K160" s="35" t="s">
         <v>942</v>
@@ -17858,9 +19280,11 @@
         <v>1341</v>
       </c>
       <c r="H161" s="50" t="s">
-        <v>1553</v>
-      </c>
-      <c r="I161" s="35"/>
+        <v>1535</v>
+      </c>
+      <c r="I161" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J161" s="35"/>
       <c r="K161" s="35" t="s">
         <v>942</v>
@@ -17916,9 +19340,11 @@
         <v>1342</v>
       </c>
       <c r="H162" s="50" t="s">
-        <v>1554</v>
-      </c>
-      <c r="I162" s="35"/>
+        <v>1702</v>
+      </c>
+      <c r="I162" s="35" t="s">
+        <v>1711</v>
+      </c>
       <c r="J162" s="35"/>
       <c r="K162" s="35" t="s">
         <v>942</v>
@@ -17974,9 +19400,11 @@
         <v>1343</v>
       </c>
       <c r="H163" s="50" t="s">
-        <v>1555</v>
-      </c>
-      <c r="I163" s="35"/>
+        <v>1536</v>
+      </c>
+      <c r="I163" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J163" s="35" t="s">
         <v>934</v>
       </c>
@@ -18030,9 +19458,11 @@
         <v>1344</v>
       </c>
       <c r="H164" s="50" t="s">
-        <v>1556</v>
-      </c>
-      <c r="I164" s="35"/>
+        <v>1537</v>
+      </c>
+      <c r="I164" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J164" s="35" t="s">
         <v>934</v>
       </c>
@@ -18086,9 +19516,11 @@
         <v>1345</v>
       </c>
       <c r="H165" s="50" t="s">
-        <v>1557</v>
-      </c>
-      <c r="I165" s="35"/>
+        <v>1538</v>
+      </c>
+      <c r="I165" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J165" s="35" t="s">
         <v>934</v>
       </c>
@@ -18142,9 +19574,11 @@
         <v>1346</v>
       </c>
       <c r="H166" s="50" t="s">
-        <v>1558</v>
-      </c>
-      <c r="I166" s="35"/>
+        <v>1539</v>
+      </c>
+      <c r="I166" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J166" s="35"/>
       <c r="K166" s="35" t="s">
         <v>942</v>
@@ -18200,9 +19634,11 @@
         <v>1345</v>
       </c>
       <c r="H167" s="50" t="s">
-        <v>1557</v>
-      </c>
-      <c r="I167" s="35"/>
+        <v>1538</v>
+      </c>
+      <c r="I167" s="35" t="s">
+        <v>1703</v>
+      </c>
       <c r="J167" s="35"/>
       <c r="K167" s="35" t="s">
         <v>942</v>
@@ -18258,9 +19694,11 @@
         <v>1347</v>
       </c>
       <c r="H168" s="50" t="s">
-        <v>1559</v>
-      </c>
-      <c r="I168" s="35"/>
+        <v>1540</v>
+      </c>
+      <c r="I168" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J168" s="35" t="s">
         <v>934</v>
       </c>
@@ -18314,9 +19752,11 @@
         <v>1348</v>
       </c>
       <c r="H169" s="50" t="s">
-        <v>1560</v>
-      </c>
-      <c r="I169" s="35"/>
+        <v>1541</v>
+      </c>
+      <c r="I169" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J169" s="35" t="s">
         <v>934</v>
       </c>
@@ -18370,9 +19810,11 @@
         <v>1349</v>
       </c>
       <c r="H170" s="50" t="s">
-        <v>1561</v>
-      </c>
-      <c r="I170" s="35"/>
+        <v>1542</v>
+      </c>
+      <c r="I170" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J170" s="35"/>
       <c r="K170" s="35" t="s">
         <v>942</v>
@@ -18428,9 +19870,11 @@
         <v>1350</v>
       </c>
       <c r="H171" s="50" t="s">
-        <v>1562</v>
-      </c>
-      <c r="I171" s="35"/>
+        <v>1704</v>
+      </c>
+      <c r="I171" s="35" t="s">
+        <v>1706</v>
+      </c>
       <c r="J171" s="35"/>
       <c r="K171" s="35" t="s">
         <v>942</v>
@@ -18486,9 +19930,11 @@
         <v>1351</v>
       </c>
       <c r="H172" s="50" t="s">
-        <v>1563</v>
-      </c>
-      <c r="I172" s="35"/>
+        <v>1705</v>
+      </c>
+      <c r="I172" s="35" t="s">
+        <v>1707</v>
+      </c>
       <c r="J172" s="35"/>
       <c r="K172" s="35" t="s">
         <v>942</v>
@@ -18544,9 +19990,11 @@
         <v>1352</v>
       </c>
       <c r="H173" s="50" t="s">
-        <v>1564</v>
-      </c>
-      <c r="I173" s="35"/>
+        <v>1708</v>
+      </c>
+      <c r="I173" s="35" t="s">
+        <v>1709</v>
+      </c>
       <c r="J173" s="35"/>
       <c r="K173" s="35" t="s">
         <v>942</v>
@@ -18602,9 +20050,11 @@
         <v>1353</v>
       </c>
       <c r="H174" s="50" t="s">
-        <v>1565</v>
-      </c>
-      <c r="I174" s="35"/>
+        <v>1543</v>
+      </c>
+      <c r="I174" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J174" s="35" t="s">
         <v>934</v>
       </c>
@@ -18658,9 +20108,11 @@
         <v>1354</v>
       </c>
       <c r="H175" s="50" t="s">
-        <v>1566</v>
-      </c>
-      <c r="I175" s="35"/>
+        <v>1544</v>
+      </c>
+      <c r="I175" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J175" s="35"/>
       <c r="K175" s="35" t="s">
         <v>942</v>
@@ -18716,9 +20168,11 @@
         <v>1355</v>
       </c>
       <c r="H176" s="50" t="s">
-        <v>1567</v>
-      </c>
-      <c r="I176" s="35"/>
+        <v>1710</v>
+      </c>
+      <c r="I176" s="35" t="s">
+        <v>1712</v>
+      </c>
       <c r="J176" s="35"/>
       <c r="K176" s="35" t="s">
         <v>942</v>
@@ -18774,9 +20228,11 @@
         <v>1356</v>
       </c>
       <c r="H177" s="50" t="s">
-        <v>1568</v>
-      </c>
-      <c r="I177" s="35"/>
+        <v>1713</v>
+      </c>
+      <c r="I177" s="35" t="s">
+        <v>1714</v>
+      </c>
       <c r="J177" s="35"/>
       <c r="K177" s="35" t="s">
         <v>942</v>
@@ -18832,9 +20288,11 @@
         <v>1357</v>
       </c>
       <c r="H178" s="50" t="s">
-        <v>1569</v>
-      </c>
-      <c r="I178" s="35"/>
+        <v>1545</v>
+      </c>
+      <c r="I178" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J178" s="35" t="s">
         <v>934</v>
       </c>
@@ -18888,9 +20346,11 @@
         <v>1358</v>
       </c>
       <c r="H179" s="50" t="s">
-        <v>1570</v>
-      </c>
-      <c r="I179" s="35"/>
+        <v>1546</v>
+      </c>
+      <c r="I179" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J179" s="35"/>
       <c r="K179" s="35" t="s">
         <v>942</v>
@@ -18946,9 +20406,11 @@
         <v>1359</v>
       </c>
       <c r="H180" s="50" t="s">
-        <v>1571</v>
-      </c>
-      <c r="I180" s="35"/>
+        <v>1547</v>
+      </c>
+      <c r="I180" s="35" t="s">
+        <v>1715</v>
+      </c>
       <c r="J180" s="35"/>
       <c r="K180" s="35" t="s">
         <v>942</v>
@@ -19004,9 +20466,11 @@
         <v>1360</v>
       </c>
       <c r="H181" s="50" t="s">
-        <v>1572</v>
-      </c>
-      <c r="I181" s="35"/>
+        <v>1548</v>
+      </c>
+      <c r="I181" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J181" s="33" t="s">
         <v>685</v>
       </c>
@@ -19060,9 +20524,11 @@
         <v>1361</v>
       </c>
       <c r="H182" s="50" t="s">
-        <v>1573</v>
-      </c>
-      <c r="I182" s="35"/>
+        <v>1549</v>
+      </c>
+      <c r="I182" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J182" s="35"/>
       <c r="K182" s="35" t="s">
         <v>942</v>
@@ -19098,7 +20564,7 @@
       <c r="AF182" s="34"/>
       <c r="AG182" s="34"/>
     </row>
-    <row r="183" spans="2:33" s="20" customFormat="1" ht="48.5" customHeight="1">
+    <row r="183" spans="2:33" s="20" customFormat="1" ht="102">
       <c r="B183" s="29" t="s">
         <v>996</v>
       </c>
@@ -19118,9 +20584,11 @@
         <v>1362</v>
       </c>
       <c r="H183" s="50" t="s">
-        <v>1574</v>
-      </c>
-      <c r="I183" s="35"/>
+        <v>1716</v>
+      </c>
+      <c r="I183" s="35" t="s">
+        <v>1717</v>
+      </c>
       <c r="J183" s="35"/>
       <c r="K183" s="35" t="s">
         <v>942</v>
@@ -19176,9 +20644,11 @@
         <v>1363</v>
       </c>
       <c r="H184" s="50" t="s">
-        <v>1575</v>
-      </c>
-      <c r="I184" s="35"/>
+        <v>1550</v>
+      </c>
+      <c r="I184" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J184" s="35"/>
       <c r="K184" s="35" t="s">
         <v>942</v>
@@ -19234,9 +20704,11 @@
         <v>1364</v>
       </c>
       <c r="H185" s="50" t="s">
-        <v>1576</v>
-      </c>
-      <c r="I185" s="35"/>
+        <v>1718</v>
+      </c>
+      <c r="I185" s="35" t="s">
+        <v>1719</v>
+      </c>
       <c r="J185" s="35"/>
       <c r="K185" s="35" t="s">
         <v>942</v>
@@ -19292,9 +20764,11 @@
         <v>1365</v>
       </c>
       <c r="H186" s="50" t="s">
-        <v>1577</v>
-      </c>
-      <c r="I186" s="35"/>
+        <v>1551</v>
+      </c>
+      <c r="I186" s="55" t="s">
+        <v>912</v>
+      </c>
       <c r="J186" s="35"/>
       <c r="K186" s="35" t="s">
         <v>942</v>
@@ -19350,9 +20824,11 @@
         <v>1366</v>
       </c>
       <c r="H187" s="50" t="s">
-        <v>1578</v>
-      </c>
-      <c r="I187" s="35"/>
+        <v>1720</v>
+      </c>
+      <c r="I187" s="35" t="s">
+        <v>1721</v>
+      </c>
       <c r="J187" s="35"/>
       <c r="K187" s="35" t="s">
         <v>942</v>
@@ -19408,9 +20884,11 @@
         <v>1367</v>
       </c>
       <c r="H188" s="50" t="s">
-        <v>1579</v>
-      </c>
-      <c r="I188" s="35"/>
+        <v>1552</v>
+      </c>
+      <c r="I188" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J188" s="35"/>
       <c r="K188" s="35" t="s">
         <v>942</v>
@@ -19466,9 +20944,11 @@
         <v>1368</v>
       </c>
       <c r="H189" s="50" t="s">
-        <v>1580</v>
-      </c>
-      <c r="I189" s="35"/>
+        <v>1722</v>
+      </c>
+      <c r="I189" s="35" t="s">
+        <v>1723</v>
+      </c>
       <c r="J189" s="35"/>
       <c r="K189" s="35" t="s">
         <v>942</v>
@@ -19524,9 +21004,11 @@
         <v>1369</v>
       </c>
       <c r="H190" s="50" t="s">
-        <v>1581</v>
-      </c>
-      <c r="I190" s="35"/>
+        <v>1553</v>
+      </c>
+      <c r="I190" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J190" s="35"/>
       <c r="K190" s="35" t="s">
         <v>942</v>
@@ -19582,9 +21064,11 @@
         <v>1370</v>
       </c>
       <c r="H191" s="50" t="s">
-        <v>1582</v>
-      </c>
-      <c r="I191" s="35"/>
+        <v>1724</v>
+      </c>
+      <c r="I191" s="35" t="s">
+        <v>1725</v>
+      </c>
       <c r="J191" s="35"/>
       <c r="K191" s="35" t="s">
         <v>942</v>
@@ -19640,9 +21124,11 @@
         <v>1371</v>
       </c>
       <c r="H192" s="50" t="s">
-        <v>1583</v>
-      </c>
-      <c r="I192" s="35"/>
+        <v>1554</v>
+      </c>
+      <c r="I192" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J192" s="35"/>
       <c r="K192" s="35" t="s">
         <v>942</v>
@@ -19698,9 +21184,11 @@
         <v>1372</v>
       </c>
       <c r="H193" s="50" t="s">
-        <v>1584</v>
-      </c>
-      <c r="I193" s="35"/>
+        <v>1726</v>
+      </c>
+      <c r="I193" s="35" t="s">
+        <v>1727</v>
+      </c>
       <c r="J193" s="35"/>
       <c r="K193" s="35" t="s">
         <v>942</v>
@@ -19756,9 +21244,11 @@
         <v>1373</v>
       </c>
       <c r="H194" s="50" t="s">
-        <v>1585</v>
-      </c>
-      <c r="I194" s="35"/>
+        <v>1555</v>
+      </c>
+      <c r="I194" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J194" s="35"/>
       <c r="K194" s="35" t="s">
         <v>942</v>
@@ -19814,9 +21304,11 @@
         <v>1374</v>
       </c>
       <c r="H195" s="50" t="s">
-        <v>1586</v>
-      </c>
-      <c r="I195" s="35"/>
+        <v>1728</v>
+      </c>
+      <c r="I195" s="35" t="s">
+        <v>1729</v>
+      </c>
       <c r="J195" s="35"/>
       <c r="K195" s="35" t="s">
         <v>942</v>
@@ -19872,9 +21364,11 @@
         <v>1375</v>
       </c>
       <c r="H196" s="50" t="s">
-        <v>1587</v>
-      </c>
-      <c r="I196" s="35"/>
+        <v>1556</v>
+      </c>
+      <c r="I196" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J196" s="35"/>
       <c r="K196" s="35" t="s">
         <v>942</v>
@@ -19930,9 +21424,11 @@
         <v>1376</v>
       </c>
       <c r="H197" s="50" t="s">
-        <v>1588</v>
-      </c>
-      <c r="I197" s="35"/>
+        <v>1730</v>
+      </c>
+      <c r="I197" s="35" t="s">
+        <v>1731</v>
+      </c>
       <c r="J197" s="35"/>
       <c r="K197" s="35" t="s">
         <v>942</v>
@@ -19988,9 +21484,11 @@
         <v>1377</v>
       </c>
       <c r="H198" s="50" t="s">
-        <v>1589</v>
-      </c>
-      <c r="I198" s="35"/>
+        <v>1557</v>
+      </c>
+      <c r="I198" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J198" s="35"/>
       <c r="K198" s="35" t="s">
         <v>942</v>
@@ -20046,9 +21544,11 @@
         <v>1378</v>
       </c>
       <c r="H199" s="50" t="s">
-        <v>1590</v>
-      </c>
-      <c r="I199" s="35"/>
+        <v>1732</v>
+      </c>
+      <c r="I199" s="35" t="s">
+        <v>1733</v>
+      </c>
       <c r="J199" s="35"/>
       <c r="K199" s="35" t="s">
         <v>942</v>
@@ -20104,9 +21604,11 @@
         <v>1379</v>
       </c>
       <c r="H200" s="50" t="s">
-        <v>1591</v>
-      </c>
-      <c r="I200" s="35"/>
+        <v>1558</v>
+      </c>
+      <c r="I200" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J200" s="35"/>
       <c r="K200" s="35" t="s">
         <v>942</v>
@@ -20162,9 +21664,11 @@
         <v>1380</v>
       </c>
       <c r="H201" s="50" t="s">
-        <v>1592</v>
-      </c>
-      <c r="I201" s="35"/>
+        <v>1734</v>
+      </c>
+      <c r="I201" s="35" t="s">
+        <v>1735</v>
+      </c>
       <c r="J201" s="35"/>
       <c r="K201" s="35" t="s">
         <v>942</v>
@@ -20220,9 +21724,11 @@
         <v>1381</v>
       </c>
       <c r="H202" s="50" t="s">
-        <v>1593</v>
-      </c>
-      <c r="I202" s="35"/>
+        <v>1559</v>
+      </c>
+      <c r="I202" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J202" s="35"/>
       <c r="K202" s="35" t="s">
         <v>942</v>
@@ -20278,9 +21784,11 @@
         <v>1382</v>
       </c>
       <c r="H203" s="50" t="s">
-        <v>1594</v>
-      </c>
-      <c r="I203" s="35"/>
+        <v>1736</v>
+      </c>
+      <c r="I203" s="35" t="s">
+        <v>1737</v>
+      </c>
       <c r="J203" s="35"/>
       <c r="K203" s="35" t="s">
         <v>942</v>
@@ -20336,9 +21844,11 @@
         <v>1383</v>
       </c>
       <c r="H204" s="50" t="s">
-        <v>1595</v>
-      </c>
-      <c r="I204" s="35"/>
+        <v>1560</v>
+      </c>
+      <c r="I204" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J204" s="35"/>
       <c r="K204" s="35" t="s">
         <v>942</v>
@@ -20394,9 +21904,11 @@
         <v>1384</v>
       </c>
       <c r="H205" s="50" t="s">
-        <v>1596</v>
-      </c>
-      <c r="I205" s="35"/>
+        <v>1738</v>
+      </c>
+      <c r="I205" s="56" t="s">
+        <v>1742</v>
+      </c>
       <c r="J205" s="35"/>
       <c r="K205" s="35" t="s">
         <v>942</v>
@@ -20452,9 +21964,11 @@
         <v>1385</v>
       </c>
       <c r="H206" s="50" t="s">
-        <v>1597</v>
-      </c>
-      <c r="I206" s="35"/>
+        <v>1561</v>
+      </c>
+      <c r="I206" s="56" t="s">
+        <v>912</v>
+      </c>
       <c r="J206" s="35"/>
       <c r="K206" s="35" t="s">
         <v>942</v>
@@ -20510,9 +22024,11 @@
         <v>1386</v>
       </c>
       <c r="H207" s="50" t="s">
-        <v>1598</v>
-      </c>
-      <c r="I207" s="35"/>
+        <v>1739</v>
+      </c>
+      <c r="I207" s="56" t="s">
+        <v>1743</v>
+      </c>
       <c r="J207" s="35"/>
       <c r="K207" s="35" t="s">
         <v>942</v>
@@ -20568,9 +22084,11 @@
         <v>1387</v>
       </c>
       <c r="H208" s="50" t="s">
-        <v>1599</v>
-      </c>
-      <c r="I208" s="35"/>
+        <v>1562</v>
+      </c>
+      <c r="I208" s="56" t="s">
+        <v>912</v>
+      </c>
       <c r="J208" s="35"/>
       <c r="K208" s="35" t="s">
         <v>942</v>
@@ -20626,9 +22144,11 @@
         <v>1388</v>
       </c>
       <c r="H209" s="50" t="s">
-        <v>1600</v>
-      </c>
-      <c r="I209" s="35"/>
+        <v>1740</v>
+      </c>
+      <c r="I209" s="56" t="s">
+        <v>1744</v>
+      </c>
       <c r="J209" s="35"/>
       <c r="K209" s="35" t="s">
         <v>942</v>
@@ -20684,9 +22204,11 @@
         <v>1389</v>
       </c>
       <c r="H210" s="50" t="s">
-        <v>1601</v>
-      </c>
-      <c r="I210" s="35"/>
+        <v>1563</v>
+      </c>
+      <c r="I210" s="56" t="s">
+        <v>912</v>
+      </c>
       <c r="J210" s="35"/>
       <c r="K210" s="35" t="s">
         <v>942</v>
@@ -20742,9 +22264,11 @@
         <v>1390</v>
       </c>
       <c r="H211" s="50" t="s">
-        <v>1602</v>
-      </c>
-      <c r="I211" s="35"/>
+        <v>1741</v>
+      </c>
+      <c r="I211" s="56" t="s">
+        <v>1745</v>
+      </c>
       <c r="J211" s="35"/>
       <c r="K211" s="35" t="s">
         <v>942</v>
@@ -20800,9 +22324,11 @@
         <v>1391</v>
       </c>
       <c r="H212" s="50" t="s">
-        <v>1603</v>
-      </c>
-      <c r="I212" s="35"/>
+        <v>1564</v>
+      </c>
+      <c r="I212" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J212" s="35"/>
       <c r="K212" s="35" t="s">
         <v>942</v>
@@ -20858,9 +22384,11 @@
         <v>1392</v>
       </c>
       <c r="H213" s="50" t="s">
-        <v>1604</v>
-      </c>
-      <c r="I213" s="35"/>
+        <v>1746</v>
+      </c>
+      <c r="I213" s="56" t="s">
+        <v>1747</v>
+      </c>
       <c r="J213" s="35"/>
       <c r="K213" s="35" t="s">
         <v>942</v>
@@ -20916,9 +22444,11 @@
         <v>1393</v>
       </c>
       <c r="H214" s="50" t="s">
-        <v>1605</v>
-      </c>
-      <c r="I214" s="35"/>
+        <v>1565</v>
+      </c>
+      <c r="I214" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J214" s="35"/>
       <c r="K214" s="35" t="s">
         <v>942</v>
@@ -20974,9 +22504,11 @@
         <v>1394</v>
       </c>
       <c r="H215" s="50" t="s">
-        <v>1606</v>
-      </c>
-      <c r="I215" s="35"/>
+        <v>1748</v>
+      </c>
+      <c r="I215" s="57" t="s">
+        <v>1749</v>
+      </c>
       <c r="J215" s="35"/>
       <c r="K215" s="35" t="s">
         <v>942</v>
@@ -21032,9 +22564,11 @@
         <v>1395</v>
       </c>
       <c r="H216" s="50" t="s">
-        <v>1607</v>
-      </c>
-      <c r="I216" s="35"/>
+        <v>1566</v>
+      </c>
+      <c r="I216" s="58" t="s">
+        <v>912</v>
+      </c>
       <c r="J216" s="35"/>
       <c r="K216" s="35" t="s">
         <v>942</v>
@@ -21090,9 +22624,11 @@
         <v>1396</v>
       </c>
       <c r="H217" s="50" t="s">
-        <v>1608</v>
-      </c>
-      <c r="I217" s="35"/>
+        <v>1750</v>
+      </c>
+      <c r="I217" s="57" t="s">
+        <v>1751</v>
+      </c>
       <c r="J217" s="35"/>
       <c r="K217" s="35" t="s">
         <v>942</v>
@@ -21148,9 +22684,11 @@
         <v>1397</v>
       </c>
       <c r="H218" s="50" t="s">
-        <v>1609</v>
-      </c>
-      <c r="I218" s="35"/>
+        <v>1567</v>
+      </c>
+      <c r="I218" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J218" s="35"/>
       <c r="K218" s="35" t="s">
         <v>942</v>
@@ -21206,9 +22744,11 @@
         <v>1398</v>
       </c>
       <c r="H219" s="50" t="s">
-        <v>1610</v>
-      </c>
-      <c r="I219" s="35"/>
+        <v>1752</v>
+      </c>
+      <c r="I219" s="57" t="s">
+        <v>1753</v>
+      </c>
       <c r="J219" s="35"/>
       <c r="K219" s="35" t="s">
         <v>942</v>
@@ -21264,9 +22804,11 @@
         <v>1399</v>
       </c>
       <c r="H220" s="50" t="s">
-        <v>1611</v>
-      </c>
-      <c r="I220" s="35"/>
+        <v>1568</v>
+      </c>
+      <c r="I220" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J220" s="35"/>
       <c r="K220" s="35" t="s">
         <v>942</v>
@@ -21322,9 +22864,11 @@
         <v>1400</v>
       </c>
       <c r="H221" s="50" t="s">
-        <v>1612</v>
-      </c>
-      <c r="I221" s="35"/>
+        <v>1754</v>
+      </c>
+      <c r="I221" s="35" t="s">
+        <v>1755</v>
+      </c>
       <c r="J221" s="35"/>
       <c r="K221" s="35" t="s">
         <v>942</v>
@@ -21380,9 +22924,11 @@
         <v>1401</v>
       </c>
       <c r="H222" s="50" t="s">
-        <v>1613</v>
-      </c>
-      <c r="I222" s="35"/>
+        <v>1569</v>
+      </c>
+      <c r="I222" s="35" t="s">
+        <v>1756</v>
+      </c>
       <c r="J222" s="35"/>
       <c r="K222" s="35" t="s">
         <v>942</v>
@@ -21438,9 +22984,11 @@
         <v>1402</v>
       </c>
       <c r="H223" s="50" t="s">
-        <v>1614</v>
-      </c>
-      <c r="I223" s="35"/>
+        <v>1757</v>
+      </c>
+      <c r="I223" s="35" t="s">
+        <v>1758</v>
+      </c>
       <c r="J223" s="35"/>
       <c r="K223" s="35" t="s">
         <v>942</v>
@@ -21496,9 +23044,11 @@
         <v>1403</v>
       </c>
       <c r="H224" s="50" t="s">
-        <v>1615</v>
-      </c>
-      <c r="I224" s="35"/>
+        <v>1570</v>
+      </c>
+      <c r="I224" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J224" s="35"/>
       <c r="K224" s="35" t="s">
         <v>942</v>
@@ -21554,9 +23104,11 @@
         <v>1404</v>
       </c>
       <c r="H225" s="50" t="s">
-        <v>1616</v>
-      </c>
-      <c r="I225" s="35"/>
+        <v>1759</v>
+      </c>
+      <c r="I225" s="57" t="s">
+        <v>1761</v>
+      </c>
       <c r="J225" s="35"/>
       <c r="K225" s="35" t="s">
         <v>942</v>
@@ -21612,9 +23164,11 @@
         <v>1405</v>
       </c>
       <c r="H226" s="50" t="s">
-        <v>1617</v>
-      </c>
-      <c r="I226" s="35"/>
+        <v>1571</v>
+      </c>
+      <c r="I226" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J226" s="35"/>
       <c r="K226" s="35" t="s">
         <v>942</v>
@@ -21670,9 +23224,11 @@
         <v>1406</v>
       </c>
       <c r="H227" s="50" t="s">
-        <v>1618</v>
-      </c>
-      <c r="I227" s="35"/>
+        <v>1760</v>
+      </c>
+      <c r="I227" s="57" t="s">
+        <v>1762</v>
+      </c>
       <c r="J227" s="35"/>
       <c r="K227" s="35" t="s">
         <v>942</v>
@@ -21728,9 +23284,11 @@
         <v>1407</v>
       </c>
       <c r="H228" s="50" t="s">
-        <v>1619</v>
-      </c>
-      <c r="I228" s="35"/>
+        <v>1572</v>
+      </c>
+      <c r="I228" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J228" s="35"/>
       <c r="K228" s="35" t="s">
         <v>942</v>
@@ -21786,9 +23344,11 @@
         <v>1408</v>
       </c>
       <c r="H229" s="50" t="s">
-        <v>1620</v>
-      </c>
-      <c r="I229" s="35"/>
+        <v>1763</v>
+      </c>
+      <c r="I229" s="57" t="s">
+        <v>1764</v>
+      </c>
       <c r="J229" s="35"/>
       <c r="K229" s="35" t="s">
         <v>942</v>
@@ -21844,9 +23404,11 @@
         <v>1409</v>
       </c>
       <c r="H230" s="50" t="s">
-        <v>1621</v>
-      </c>
-      <c r="I230" s="35"/>
+        <v>1573</v>
+      </c>
+      <c r="I230" s="59" t="s">
+        <v>912</v>
+      </c>
       <c r="J230" s="35"/>
       <c r="K230" s="35" t="s">
         <v>942</v>
@@ -21902,9 +23464,11 @@
         <v>1410</v>
       </c>
       <c r="H231" s="50" t="s">
-        <v>1622</v>
-      </c>
-      <c r="I231" s="35"/>
+        <v>1765</v>
+      </c>
+      <c r="I231" s="57" t="s">
+        <v>1766</v>
+      </c>
       <c r="J231" s="35"/>
       <c r="K231" s="35" t="s">
         <v>942</v>
@@ -21960,9 +23524,11 @@
         <v>1411</v>
       </c>
       <c r="H232" s="50" t="s">
-        <v>1623</v>
-      </c>
-      <c r="I232" s="35"/>
+        <v>1574</v>
+      </c>
+      <c r="I232" s="58" t="s">
+        <v>912</v>
+      </c>
       <c r="J232" s="35"/>
       <c r="K232" s="35" t="s">
         <v>942</v>
@@ -22018,9 +23584,11 @@
         <v>1412</v>
       </c>
       <c r="H233" s="50" t="s">
-        <v>1624</v>
-      </c>
-      <c r="I233" s="35"/>
+        <v>1767</v>
+      </c>
+      <c r="I233" s="57" t="s">
+        <v>1768</v>
+      </c>
       <c r="J233" s="35"/>
       <c r="K233" s="35" t="s">
         <v>942</v>
@@ -22076,9 +23644,11 @@
         <v>1413</v>
       </c>
       <c r="H234" s="50" t="s">
-        <v>1625</v>
-      </c>
-      <c r="I234" s="35"/>
+        <v>1575</v>
+      </c>
+      <c r="I234" s="58" t="s">
+        <v>912</v>
+      </c>
       <c r="J234" s="35"/>
       <c r="K234" s="35" t="s">
         <v>942</v>
@@ -22134,9 +23704,11 @@
         <v>1414</v>
       </c>
       <c r="H235" s="50" t="s">
-        <v>1626</v>
-      </c>
-      <c r="I235" s="35"/>
+        <v>1576</v>
+      </c>
+      <c r="I235" s="57" t="s">
+        <v>1769</v>
+      </c>
       <c r="J235" s="35"/>
       <c r="K235" s="35" t="s">
         <v>942</v>
@@ -22192,9 +23764,11 @@
         <v>1415</v>
       </c>
       <c r="H236" s="50" t="s">
-        <v>1627</v>
-      </c>
-      <c r="I236" s="35"/>
+        <v>1577</v>
+      </c>
+      <c r="I236" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J236" s="35"/>
       <c r="K236" s="35" t="s">
         <v>942</v>
@@ -22250,9 +23824,11 @@
         <v>1416</v>
       </c>
       <c r="H237" s="50" t="s">
-        <v>1628</v>
-      </c>
-      <c r="I237" s="35"/>
+        <v>1770</v>
+      </c>
+      <c r="I237" s="57" t="s">
+        <v>1771</v>
+      </c>
       <c r="J237" s="35"/>
       <c r="K237" s="35" t="s">
         <v>942</v>
@@ -22308,9 +23884,11 @@
         <v>1417</v>
       </c>
       <c r="H238" s="50" t="s">
-        <v>1629</v>
-      </c>
-      <c r="I238" s="35"/>
+        <v>1578</v>
+      </c>
+      <c r="I238" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J238" s="35"/>
       <c r="K238" s="35" t="s">
         <v>942</v>
@@ -22366,9 +23944,11 @@
         <v>1418</v>
       </c>
       <c r="H239" s="50" t="s">
-        <v>1630</v>
-      </c>
-      <c r="I239" s="35"/>
+        <v>1772</v>
+      </c>
+      <c r="I239" s="57" t="s">
+        <v>1773</v>
+      </c>
       <c r="J239" s="35"/>
       <c r="K239" s="35" t="s">
         <v>942</v>
@@ -22424,9 +24004,11 @@
         <v>1419</v>
       </c>
       <c r="H240" s="50" t="s">
-        <v>1631</v>
-      </c>
-      <c r="I240" s="35"/>
+        <v>1579</v>
+      </c>
+      <c r="I240" s="35" t="s">
+        <v>1774</v>
+      </c>
       <c r="J240" s="35"/>
       <c r="K240" s="35" t="s">
         <v>942</v>
@@ -22482,9 +24064,11 @@
         <v>1420</v>
       </c>
       <c r="H241" s="50" t="s">
-        <v>1632</v>
-      </c>
-      <c r="I241" s="35"/>
+        <v>1580</v>
+      </c>
+      <c r="I241" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J241" s="35"/>
       <c r="K241" s="35" t="s">
         <v>942</v>
@@ -22540,9 +24124,11 @@
         <v>1421</v>
       </c>
       <c r="H242" s="50" t="s">
-        <v>1633</v>
-      </c>
-      <c r="I242" s="35"/>
+        <v>1581</v>
+      </c>
+      <c r="I242" s="57" t="s">
+        <v>1775</v>
+      </c>
       <c r="J242" s="35"/>
       <c r="K242" s="35" t="s">
         <v>942</v>
@@ -22598,9 +24184,11 @@
         <v>1422</v>
       </c>
       <c r="H243" s="50" t="s">
-        <v>1634</v>
-      </c>
-      <c r="I243" s="35"/>
+        <v>1582</v>
+      </c>
+      <c r="I243" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J243" s="35"/>
       <c r="K243" s="35" t="s">
         <v>942</v>
@@ -22656,9 +24244,11 @@
         <v>1423</v>
       </c>
       <c r="H244" s="50" t="s">
-        <v>1635</v>
-      </c>
-      <c r="I244" s="35"/>
+        <v>1776</v>
+      </c>
+      <c r="I244" s="57" t="s">
+        <v>1778</v>
+      </c>
       <c r="J244" s="35"/>
       <c r="K244" s="35" t="s">
         <v>942</v>
@@ -22714,9 +24304,11 @@
         <v>1424</v>
       </c>
       <c r="H245" s="50" t="s">
-        <v>1636</v>
-      </c>
-      <c r="I245" s="35"/>
+        <v>1583</v>
+      </c>
+      <c r="I245" s="35" t="s">
+        <v>912</v>
+      </c>
       <c r="J245" s="35"/>
       <c r="K245" s="35" t="s">
         <v>942</v>
@@ -22772,9 +24364,11 @@
         <v>1425</v>
       </c>
       <c r="H246" s="50" t="s">
-        <v>1637</v>
-      </c>
-      <c r="I246" s="35"/>
+        <v>1777</v>
+      </c>
+      <c r="I246" s="57" t="s">
+        <v>1779</v>
+      </c>
       <c r="J246" s="35"/>
       <c r="K246" s="35" t="s">
         <v>942</v>
@@ -40056,7 +41650,7 @@
         <v>531</v>
       </c>
       <c r="J411" s="35" t="s">
-        <v>1696</v>
+        <v>1642</v>
       </c>
       <c r="K411" s="33" t="s">
         <v>658</v>
@@ -44105,11 +45699,11 @@
   </sheetPr>
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="23" customHeight="1"/>
@@ -44216,7 +45810,7 @@
     </row>
     <row r="13" spans="1:2" ht="18.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>1638</v>
+        <v>1584</v>
       </c>
       <c r="B13" s="22">
         <v>11</v>
@@ -44232,7 +45826,7 @@
     </row>
     <row r="15" spans="1:2" ht="18.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>1643</v>
+        <v>1589</v>
       </c>
       <c r="B15" s="22">
         <v>13</v>
@@ -44416,7 +46010,7 @@
     </row>
     <row r="38" spans="1:2" ht="18.25" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>1673</v>
+        <v>1619</v>
       </c>
       <c r="B38" s="22">
         <v>36</v>

</xml_diff>

<commit_message>
update to apply gihou and daien operation
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ty/ruby/zakuro/doc/operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD500E6-F44F-9549-91BF-33F537148D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE835286-EFF5-3546-AE4A-D4AB3DD42C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="31920" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10533" uniqueCount="1896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10726" uniqueCount="1896">
   <si>
     <t>ID</t>
   </si>
@@ -10122,10 +10122,10 @@
   <dimension ref="A1:AG447"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AD2" sqref="AD2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="20" customHeight="1"/>
@@ -10489,7 +10489,9 @@
       <c r="I4" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J4" s="31"/>
+      <c r="J4" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K4" s="33" t="s">
         <v>942</v>
       </c>
@@ -10592,7 +10594,9 @@
       <c r="I5" s="33" t="s">
         <v>1581</v>
       </c>
-      <c r="J5" s="31"/>
+      <c r="J5" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K5" s="33" t="s">
         <v>942</v>
       </c>
@@ -10800,7 +10804,9 @@
       <c r="I7" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J7" s="31"/>
+      <c r="J7" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K7" s="33" t="s">
         <v>942</v>
       </c>
@@ -10903,7 +10909,9 @@
       <c r="I8" s="33" t="s">
         <v>1583</v>
       </c>
-      <c r="J8" s="31"/>
+      <c r="J8" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K8" s="33" t="s">
         <v>942</v>
       </c>
@@ -11216,7 +11224,9 @@
       <c r="I11" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J11" s="31"/>
+      <c r="J11" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K11" s="33" t="s">
         <v>942</v>
       </c>
@@ -11319,7 +11329,9 @@
       <c r="I12" s="33" t="s">
         <v>1586</v>
       </c>
-      <c r="J12" s="44"/>
+      <c r="J12" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K12" s="33" t="s">
         <v>942</v>
       </c>
@@ -11422,7 +11434,9 @@
       <c r="I13" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J13" s="31"/>
+      <c r="J13" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K13" s="33" t="s">
         <v>942</v>
       </c>
@@ -11525,7 +11539,9 @@
       <c r="I14" s="33" t="s">
         <v>1791</v>
       </c>
-      <c r="J14" s="31"/>
+      <c r="J14" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K14" s="33" t="s">
         <v>942</v>
       </c>
@@ -11628,7 +11644,9 @@
       <c r="I15" s="33" t="s">
         <v>1588</v>
       </c>
-      <c r="J15" s="31"/>
+      <c r="J15" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K15" s="49" t="s">
         <v>933</v>
       </c>
@@ -12781,7 +12799,9 @@
       <c r="I26" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J26" s="31"/>
+      <c r="J26" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K26" s="33" t="s">
         <v>942</v>
       </c>
@@ -12884,7 +12904,9 @@
       <c r="I27" s="33" t="s">
         <v>1592</v>
       </c>
-      <c r="J27" s="31"/>
+      <c r="J27" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K27" s="33" t="s">
         <v>942</v>
       </c>
@@ -12987,7 +13009,9 @@
       <c r="I28" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J28" s="31"/>
+      <c r="J28" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K28" s="33" t="s">
         <v>942</v>
       </c>
@@ -13090,7 +13114,9 @@
       <c r="I29" s="33" t="s">
         <v>1594</v>
       </c>
-      <c r="J29" s="31"/>
+      <c r="J29" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K29" s="33" t="s">
         <v>942</v>
       </c>
@@ -13193,7 +13219,9 @@
       <c r="I30" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J30" s="31"/>
+      <c r="J30" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K30" s="33" t="s">
         <v>942</v>
       </c>
@@ -13296,7 +13324,9 @@
       <c r="I31" s="33" t="s">
         <v>1596</v>
       </c>
-      <c r="J31" s="31"/>
+      <c r="J31" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K31" s="33" t="s">
         <v>942</v>
       </c>
@@ -13399,7 +13429,9 @@
       <c r="I32" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J32" s="31"/>
+      <c r="J32" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K32" s="33" t="s">
         <v>942</v>
       </c>
@@ -13502,7 +13534,9 @@
       <c r="I33" s="33" t="s">
         <v>1599</v>
       </c>
-      <c r="J33" s="31"/>
+      <c r="J33" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K33" s="33" t="s">
         <v>942</v>
       </c>
@@ -13605,7 +13639,9 @@
       <c r="I34" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J34" s="31"/>
+      <c r="J34" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K34" s="33" t="s">
         <v>942</v>
       </c>
@@ -13813,7 +13849,9 @@
       <c r="I36" s="33" t="s">
         <v>1601</v>
       </c>
-      <c r="J36" s="31"/>
+      <c r="J36" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K36" s="33" t="s">
         <v>942</v>
       </c>
@@ -13916,7 +13954,9 @@
       <c r="I37" s="33" t="s">
         <v>1602</v>
       </c>
-      <c r="J37" s="31"/>
+      <c r="J37" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K37" s="33" t="s">
         <v>942</v>
       </c>
@@ -14124,7 +14164,9 @@
       <c r="I39" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J39" s="31"/>
+      <c r="J39" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K39" s="33" t="s">
         <v>942</v>
       </c>
@@ -14227,7 +14269,9 @@
       <c r="I40" s="33" t="s">
         <v>1606</v>
       </c>
-      <c r="J40" s="31"/>
+      <c r="J40" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K40" s="33" t="s">
         <v>942</v>
       </c>
@@ -14330,7 +14374,9 @@
       <c r="I41" s="33" t="s">
         <v>1607</v>
       </c>
-      <c r="J41" s="31"/>
+      <c r="J41" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K41" s="33" t="s">
         <v>942</v>
       </c>
@@ -14433,7 +14479,9 @@
       <c r="I42" s="33" t="s">
         <v>1609</v>
       </c>
-      <c r="J42" s="31"/>
+      <c r="J42" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K42" s="33" t="s">
         <v>942</v>
       </c>
@@ -14851,7 +14899,9 @@
       <c r="I46" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J46" s="33"/>
+      <c r="J46" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K46" s="33" t="s">
         <v>942</v>
       </c>
@@ -14954,7 +15004,9 @@
       <c r="I47" s="33" t="s">
         <v>1611</v>
       </c>
-      <c r="J47" s="33"/>
+      <c r="J47" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K47" s="33" t="s">
         <v>942</v>
       </c>
@@ -15162,7 +15214,9 @@
       <c r="I49" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J49" s="33"/>
+      <c r="J49" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K49" s="33" t="s">
         <v>942</v>
       </c>
@@ -15265,7 +15319,9 @@
       <c r="I50" s="33" t="s">
         <v>1613</v>
       </c>
-      <c r="J50" s="33"/>
+      <c r="J50" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K50" s="33" t="s">
         <v>942</v>
       </c>
@@ -15368,7 +15424,9 @@
       <c r="I51" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J51" s="33"/>
+      <c r="J51" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K51" s="33" t="s">
         <v>942</v>
       </c>
@@ -15471,7 +15529,9 @@
       <c r="I52" s="33" t="s">
         <v>1616</v>
       </c>
-      <c r="J52" s="33"/>
+      <c r="J52" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K52" s="33" t="s">
         <v>942</v>
       </c>
@@ -15679,7 +15739,9 @@
       <c r="I54" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J54" s="33"/>
+      <c r="J54" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K54" s="33" t="s">
         <v>942</v>
       </c>
@@ -15782,7 +15844,9 @@
       <c r="I55" s="33" t="s">
         <v>1618</v>
       </c>
-      <c r="J55" s="33"/>
+      <c r="J55" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K55" s="33" t="s">
         <v>942</v>
       </c>
@@ -15885,7 +15949,9 @@
       <c r="I56" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J56" s="33"/>
+      <c r="J56" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K56" s="33" t="s">
         <v>942</v>
       </c>
@@ -15988,7 +16054,9 @@
       <c r="I57" s="33" t="s">
         <v>1620</v>
       </c>
-      <c r="J57" s="33"/>
+      <c r="J57" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K57" s="33" t="s">
         <v>942</v>
       </c>
@@ -16091,7 +16159,9 @@
       <c r="I58" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J58" s="33"/>
+      <c r="J58" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K58" s="33" t="s">
         <v>942</v>
       </c>
@@ -16194,7 +16264,9 @@
       <c r="I59" s="33" t="s">
         <v>1767</v>
       </c>
-      <c r="J59" s="33"/>
+      <c r="J59" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K59" s="33" t="s">
         <v>942</v>
       </c>
@@ -16297,7 +16369,9 @@
       <c r="I60" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J60" s="33"/>
+      <c r="J60" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K60" s="33" t="s">
         <v>942</v>
       </c>
@@ -16400,7 +16474,9 @@
       <c r="I61" s="33" t="s">
         <v>1623</v>
       </c>
-      <c r="J61" s="33"/>
+      <c r="J61" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K61" s="33" t="s">
         <v>942</v>
       </c>
@@ -16503,7 +16579,9 @@
       <c r="I62" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J62" s="33"/>
+      <c r="J62" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K62" s="33" t="s">
         <v>942</v>
       </c>
@@ -16606,7 +16684,9 @@
       <c r="I63" s="33" t="s">
         <v>1625</v>
       </c>
-      <c r="J63" s="33"/>
+      <c r="J63" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K63" s="33" t="s">
         <v>942</v>
       </c>
@@ -16919,7 +16999,9 @@
       <c r="I66" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J66" s="33"/>
+      <c r="J66" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K66" s="33" t="s">
         <v>942</v>
       </c>
@@ -17022,7 +17104,9 @@
       <c r="I67" s="33" t="s">
         <v>1768</v>
       </c>
-      <c r="J67" s="33"/>
+      <c r="J67" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K67" s="33" t="s">
         <v>942</v>
       </c>
@@ -17125,7 +17209,9 @@
       <c r="I68" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J68" s="33"/>
+      <c r="J68" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K68" s="33" t="s">
         <v>942</v>
       </c>
@@ -17228,7 +17314,9 @@
       <c r="I69" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J69" s="33"/>
+      <c r="J69" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K69" s="33" t="s">
         <v>942</v>
       </c>
@@ -17331,7 +17419,9 @@
       <c r="I70" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J70" s="31"/>
+      <c r="J70" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K70" s="33" t="s">
         <v>942</v>
       </c>
@@ -17434,7 +17524,9 @@
       <c r="I71" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J71" s="31"/>
+      <c r="J71" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K71" s="33" t="s">
         <v>942</v>
       </c>
@@ -17537,7 +17629,9 @@
       <c r="I72" s="33" t="s">
         <v>1631</v>
       </c>
-      <c r="J72" s="31"/>
+      <c r="J72" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K72" s="33" t="s">
         <v>942</v>
       </c>
@@ -17640,7 +17734,9 @@
       <c r="I73" s="52" t="s">
         <v>912</v>
       </c>
-      <c r="J73" s="31"/>
+      <c r="J73" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K73" s="33" t="s">
         <v>942</v>
       </c>
@@ -17743,7 +17839,9 @@
       <c r="I74" s="33" t="s">
         <v>1633</v>
       </c>
-      <c r="J74" s="31"/>
+      <c r="J74" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K74" s="33" t="s">
         <v>942</v>
       </c>
@@ -17846,7 +17944,9 @@
       <c r="I75" s="33" t="s">
         <v>1634</v>
       </c>
-      <c r="J75" s="31"/>
+      <c r="J75" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K75" s="33" t="s">
         <v>942</v>
       </c>
@@ -17949,7 +18049,9 @@
       <c r="I76" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J76" s="31"/>
+      <c r="J76" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K76" s="33" t="s">
         <v>942</v>
       </c>
@@ -18157,7 +18259,9 @@
       <c r="I78" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J78" s="31"/>
+      <c r="J78" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K78" s="33" t="s">
         <v>942</v>
       </c>
@@ -18260,7 +18364,9 @@
       <c r="I79" s="33" t="s">
         <v>1639</v>
       </c>
-      <c r="J79" s="31"/>
+      <c r="J79" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K79" s="33" t="s">
         <v>942</v>
       </c>
@@ -18363,7 +18469,9 @@
       <c r="I80" s="33" t="s">
         <v>1640</v>
       </c>
-      <c r="J80" s="31"/>
+      <c r="J80" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K80" s="33" t="s">
         <v>942</v>
       </c>
@@ -18571,7 +18679,9 @@
       <c r="I82" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J82" s="31"/>
+      <c r="J82" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K82" s="33" t="s">
         <v>942</v>
       </c>
@@ -18674,7 +18784,9 @@
       <c r="I83" s="33" t="s">
         <v>1641</v>
       </c>
-      <c r="J83" s="31"/>
+      <c r="J83" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K83" s="33" t="s">
         <v>942</v>
       </c>
@@ -18777,7 +18889,9 @@
       <c r="I84" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J84" s="31"/>
+      <c r="J84" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K84" s="33" t="s">
         <v>942</v>
       </c>
@@ -18880,7 +18994,9 @@
       <c r="I85" s="33" t="s">
         <v>1642</v>
       </c>
-      <c r="J85" s="31"/>
+      <c r="J85" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K85" s="33" t="s">
         <v>942</v>
       </c>
@@ -18983,7 +19099,9 @@
       <c r="I86" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J86" s="31"/>
+      <c r="J86" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K86" s="33" t="s">
         <v>942</v>
       </c>
@@ -19086,7 +19204,9 @@
       <c r="I87" s="33" t="s">
         <v>1643</v>
       </c>
-      <c r="J87" s="31"/>
+      <c r="J87" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K87" s="33" t="s">
         <v>942</v>
       </c>
@@ -19399,7 +19519,9 @@
       <c r="I90" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J90" s="33"/>
+      <c r="J90" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K90" s="33" t="s">
         <v>942</v>
       </c>
@@ -19502,7 +19624,9 @@
       <c r="I91" s="33" t="s">
         <v>1645</v>
       </c>
-      <c r="J91" s="33"/>
+      <c r="J91" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K91" s="33" t="s">
         <v>942</v>
       </c>
@@ -19605,7 +19729,9 @@
       <c r="I92" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J92" s="33"/>
+      <c r="J92" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K92" s="33" t="s">
         <v>942</v>
       </c>
@@ -19708,7 +19834,9 @@
       <c r="I93" s="33" t="s">
         <v>1646</v>
       </c>
-      <c r="J93" s="33"/>
+      <c r="J93" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K93" s="33" t="s">
         <v>942</v>
       </c>
@@ -19811,7 +19939,9 @@
       <c r="I94" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J94" s="33"/>
+      <c r="J94" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K94" s="33" t="s">
         <v>942</v>
       </c>
@@ -19914,7 +20044,9 @@
       <c r="I95" s="33" t="s">
         <v>1647</v>
       </c>
-      <c r="J95" s="33"/>
+      <c r="J95" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K95" s="33" t="s">
         <v>942</v>
       </c>
@@ -20122,7 +20254,9 @@
       <c r="I97" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J97" s="33"/>
+      <c r="J97" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K97" s="33" t="s">
         <v>942</v>
       </c>
@@ -20225,7 +20359,9 @@
       <c r="I98" s="33" t="s">
         <v>1648</v>
       </c>
-      <c r="J98" s="33"/>
+      <c r="J98" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K98" s="33" t="s">
         <v>942</v>
       </c>
@@ -20538,7 +20674,9 @@
       <c r="I101" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J101" s="33"/>
+      <c r="J101" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K101" s="33" t="s">
         <v>942</v>
       </c>
@@ -20641,7 +20779,9 @@
       <c r="I102" s="33" t="s">
         <v>1650</v>
       </c>
-      <c r="J102" s="33"/>
+      <c r="J102" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K102" s="33" t="s">
         <v>942</v>
       </c>
@@ -20744,7 +20884,9 @@
       <c r="I103" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J103" s="33"/>
+      <c r="J103" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K103" s="33" t="s">
         <v>942</v>
       </c>
@@ -20847,7 +20989,9 @@
       <c r="I104" s="33" t="s">
         <v>1651</v>
       </c>
-      <c r="J104" s="33"/>
+      <c r="J104" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K104" s="33" t="s">
         <v>942</v>
       </c>
@@ -20950,7 +21094,9 @@
       <c r="I105" s="52" t="s">
         <v>912</v>
       </c>
-      <c r="J105" s="33"/>
+      <c r="J105" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K105" s="33" t="s">
         <v>942</v>
       </c>
@@ -21053,7 +21199,9 @@
       <c r="I106" s="33" t="s">
         <v>1653</v>
       </c>
-      <c r="J106" s="33"/>
+      <c r="J106" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K106" s="33" t="s">
         <v>942</v>
       </c>
@@ -21156,7 +21304,9 @@
       <c r="I107" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J107" s="33"/>
+      <c r="J107" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K107" s="33" t="s">
         <v>942</v>
       </c>
@@ -21259,7 +21409,9 @@
       <c r="I108" s="33" t="s">
         <v>1655</v>
       </c>
-      <c r="J108" s="33"/>
+      <c r="J108" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K108" s="33" t="s">
         <v>942</v>
       </c>
@@ -21362,7 +21514,9 @@
       <c r="I109" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J109" s="33"/>
+      <c r="J109" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K109" s="33" t="s">
         <v>942</v>
       </c>
@@ -21465,7 +21619,9 @@
       <c r="I110" s="33" t="s">
         <v>1656</v>
       </c>
-      <c r="J110" s="33"/>
+      <c r="J110" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K110" s="33" t="s">
         <v>942</v>
       </c>
@@ -21883,7 +22039,9 @@
       <c r="I114" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J114" s="33"/>
+      <c r="J114" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K114" s="33" t="s">
         <v>942</v>
       </c>
@@ -21986,7 +22144,9 @@
       <c r="I115" s="33" t="s">
         <v>1658</v>
       </c>
-      <c r="J115" s="33"/>
+      <c r="J115" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K115" s="33" t="s">
         <v>942</v>
       </c>
@@ -22089,7 +22249,9 @@
       <c r="I116" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J116" s="33"/>
+      <c r="J116" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K116" s="33" t="s">
         <v>942</v>
       </c>
@@ -22192,7 +22354,9 @@
       <c r="I117" s="33" t="s">
         <v>1659</v>
       </c>
-      <c r="J117" s="33"/>
+      <c r="J117" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K117" s="33" t="s">
         <v>942</v>
       </c>
@@ -22295,7 +22459,9 @@
       <c r="I118" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J118" s="33"/>
+      <c r="J118" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K118" s="33" t="s">
         <v>942</v>
       </c>
@@ -22398,7 +22564,9 @@
       <c r="I119" s="33" t="s">
         <v>1661</v>
       </c>
-      <c r="J119" s="33"/>
+      <c r="J119" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K119" s="33" t="s">
         <v>942</v>
       </c>
@@ -22501,7 +22669,9 @@
       <c r="I120" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J120" s="33"/>
+      <c r="J120" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K120" s="33" t="s">
         <v>942</v>
       </c>
@@ -22604,7 +22774,9 @@
       <c r="I121" s="33" t="s">
         <v>1663</v>
       </c>
-      <c r="J121" s="33"/>
+      <c r="J121" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K121" s="33" t="s">
         <v>942</v>
       </c>
@@ -22812,7 +22984,9 @@
       <c r="I123" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J123" s="33"/>
+      <c r="J123" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K123" s="33" t="s">
         <v>942</v>
       </c>
@@ -22915,7 +23089,9 @@
       <c r="I124" s="33" t="s">
         <v>1665</v>
       </c>
-      <c r="J124" s="33"/>
+      <c r="J124" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K124" s="33" t="s">
         <v>942</v>
       </c>
@@ -23018,7 +23194,9 @@
       <c r="I125" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J125" s="33"/>
+      <c r="J125" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K125" s="33" t="s">
         <v>942</v>
       </c>
@@ -23121,7 +23299,9 @@
       <c r="I126" s="33" t="s">
         <v>1770</v>
       </c>
-      <c r="J126" s="33"/>
+      <c r="J126" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K126" s="33" t="s">
         <v>942</v>
       </c>
@@ -23539,7 +23719,9 @@
       <c r="I130" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J130" s="33"/>
+      <c r="J130" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K130" s="33" t="s">
         <v>942</v>
       </c>
@@ -23642,7 +23824,9 @@
       <c r="I131" s="33" t="s">
         <v>1668</v>
       </c>
-      <c r="J131" s="33"/>
+      <c r="J131" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K131" s="33" t="s">
         <v>942</v>
       </c>
@@ -23850,7 +24034,9 @@
       <c r="I133" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J133" s="33"/>
+      <c r="J133" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K133" s="33" t="s">
         <v>942</v>
       </c>
@@ -23953,7 +24139,9 @@
       <c r="I134" s="33" t="s">
         <v>1670</v>
       </c>
-      <c r="J134" s="33"/>
+      <c r="J134" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K134" s="33" t="s">
         <v>942</v>
       </c>
@@ -24056,7 +24244,9 @@
       <c r="I135" s="33" t="s">
         <v>1671</v>
       </c>
-      <c r="J135" s="33"/>
+      <c r="J135" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K135" s="33" t="s">
         <v>942</v>
       </c>
@@ -24159,7 +24349,9 @@
       <c r="I136" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J136" s="33"/>
+      <c r="J136" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K136" s="33" t="s">
         <v>942</v>
       </c>
@@ -24262,7 +24454,9 @@
       <c r="I137" s="33" t="s">
         <v>1673</v>
       </c>
-      <c r="J137" s="33"/>
+      <c r="J137" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K137" s="33" t="s">
         <v>942</v>
       </c>
@@ -24470,7 +24664,9 @@
       <c r="I139" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J139" s="33"/>
+      <c r="J139" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K139" s="33" t="s">
         <v>942</v>
       </c>
@@ -24573,7 +24769,9 @@
       <c r="I140" s="33" t="s">
         <v>1675</v>
       </c>
-      <c r="J140" s="33"/>
+      <c r="J140" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K140" s="33" t="s">
         <v>942</v>
       </c>
@@ -24781,7 +24979,9 @@
       <c r="I142" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J142" s="33"/>
+      <c r="J142" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K142" s="33" t="s">
         <v>942</v>
       </c>
@@ -24884,7 +25084,9 @@
       <c r="I143" s="33" t="s">
         <v>1677</v>
       </c>
-      <c r="J143" s="33"/>
+      <c r="J143" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K143" s="33" t="s">
         <v>942</v>
       </c>
@@ -25092,7 +25294,9 @@
       <c r="I145" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J145" s="33"/>
+      <c r="J145" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K145" s="33" t="s">
         <v>942</v>
       </c>
@@ -25195,7 +25399,9 @@
       <c r="I146" s="33" t="s">
         <v>1679</v>
       </c>
-      <c r="J146" s="33"/>
+      <c r="J146" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K146" s="33" t="s">
         <v>942</v>
       </c>
@@ -25508,7 +25714,9 @@
       <c r="I149" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J149" s="33"/>
+      <c r="J149" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K149" s="33" t="s">
         <v>942</v>
       </c>
@@ -25611,7 +25819,9 @@
       <c r="I150" s="33" t="s">
         <v>1681</v>
       </c>
-      <c r="J150" s="33"/>
+      <c r="J150" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K150" s="33" t="s">
         <v>942</v>
       </c>
@@ -25714,7 +25924,9 @@
       <c r="I151" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J151" s="33"/>
+      <c r="J151" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K151" s="33" t="s">
         <v>942</v>
       </c>
@@ -25817,7 +26029,9 @@
       <c r="I152" s="33" t="s">
         <v>1684</v>
       </c>
-      <c r="J152" s="33"/>
+      <c r="J152" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K152" s="33" t="s">
         <v>942</v>
       </c>
@@ -25920,7 +26134,9 @@
       <c r="I153" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J153" s="33"/>
+      <c r="J153" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K153" s="33" t="s">
         <v>942</v>
       </c>
@@ -26023,7 +26239,9 @@
       <c r="I154" s="33" t="s">
         <v>1685</v>
       </c>
-      <c r="J154" s="33"/>
+      <c r="J154" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K154" s="33" t="s">
         <v>942</v>
       </c>
@@ -26126,7 +26344,9 @@
       <c r="I155" s="33" t="s">
         <v>1687</v>
       </c>
-      <c r="J155" s="33"/>
+      <c r="J155" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K155" s="33" t="s">
         <v>942</v>
       </c>
@@ -26229,7 +26449,9 @@
       <c r="I156" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J156" s="33"/>
+      <c r="J156" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K156" s="33" t="s">
         <v>942</v>
       </c>
@@ -26332,7 +26554,9 @@
       <c r="I157" s="33" t="s">
         <v>1689</v>
       </c>
-      <c r="J157" s="33"/>
+      <c r="J157" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K157" s="33" t="s">
         <v>942</v>
       </c>
@@ -26435,7 +26659,9 @@
       <c r="I158" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J158" s="33"/>
+      <c r="J158" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K158" s="33" t="s">
         <v>942</v>
       </c>
@@ -26538,7 +26764,9 @@
       <c r="I159" s="33" t="s">
         <v>1771</v>
       </c>
-      <c r="J159" s="33"/>
+      <c r="J159" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K159" s="33" t="s">
         <v>942</v>
       </c>
@@ -26641,7 +26869,9 @@
       <c r="I160" s="33" t="s">
         <v>1690</v>
       </c>
-      <c r="J160" s="33"/>
+      <c r="J160" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K160" s="33" t="s">
         <v>942</v>
       </c>
@@ -26744,7 +26974,9 @@
       <c r="I161" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J161" s="33"/>
+      <c r="J161" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K161" s="33" t="s">
         <v>942</v>
       </c>
@@ -26847,7 +27079,9 @@
       <c r="I162" s="33" t="s">
         <v>1699</v>
       </c>
-      <c r="J162" s="33"/>
+      <c r="J162" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K162" s="33" t="s">
         <v>942</v>
       </c>
@@ -27265,7 +27499,9 @@
       <c r="I166" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J166" s="33"/>
+      <c r="J166" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K166" s="33" t="s">
         <v>942</v>
       </c>
@@ -27368,7 +27604,9 @@
       <c r="I167" s="33" t="s">
         <v>1692</v>
       </c>
-      <c r="J167" s="33"/>
+      <c r="J167" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K167" s="33" t="s">
         <v>942</v>
       </c>
@@ -27681,7 +27919,9 @@
       <c r="I170" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J170" s="33"/>
+      <c r="J170" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K170" s="33" t="s">
         <v>942</v>
       </c>
@@ -27784,7 +28024,9 @@
       <c r="I171" s="33" t="s">
         <v>1695</v>
       </c>
-      <c r="J171" s="33"/>
+      <c r="J171" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K171" s="33" t="s">
         <v>942</v>
       </c>
@@ -27887,7 +28129,9 @@
       <c r="I172" s="33" t="s">
         <v>1696</v>
       </c>
-      <c r="J172" s="33"/>
+      <c r="J172" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K172" s="33" t="s">
         <v>942</v>
       </c>
@@ -27990,7 +28234,9 @@
       <c r="I173" s="33" t="s">
         <v>1774</v>
       </c>
-      <c r="J173" s="33"/>
+      <c r="J173" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K173" s="33" t="s">
         <v>942</v>
       </c>
@@ -28198,7 +28444,9 @@
       <c r="I175" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J175" s="33"/>
+      <c r="J175" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K175" s="33" t="s">
         <v>942</v>
       </c>
@@ -28301,7 +28549,9 @@
       <c r="I176" s="33" t="s">
         <v>1700</v>
       </c>
-      <c r="J176" s="33"/>
+      <c r="J176" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K176" s="33" t="s">
         <v>942</v>
       </c>
@@ -28404,7 +28654,9 @@
       <c r="I177" s="33" t="s">
         <v>1702</v>
       </c>
-      <c r="J177" s="33"/>
+      <c r="J177" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K177" s="33" t="s">
         <v>942</v>
       </c>
@@ -28612,7 +28864,9 @@
       <c r="I179" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J179" s="33"/>
+      <c r="J179" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K179" s="33" t="s">
         <v>942</v>
       </c>
@@ -28715,7 +28969,9 @@
       <c r="I180" s="33" t="s">
         <v>1775</v>
       </c>
-      <c r="J180" s="33"/>
+      <c r="J180" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K180" s="33" t="s">
         <v>942</v>
       </c>
@@ -28923,7 +29179,9 @@
       <c r="I182" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J182" s="33"/>
+      <c r="J182" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K182" s="33" t="s">
         <v>942</v>
       </c>
@@ -29026,7 +29284,9 @@
       <c r="I183" s="33" t="s">
         <v>1704</v>
       </c>
-      <c r="J183" s="33"/>
+      <c r="J183" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K183" s="33" t="s">
         <v>942</v>
       </c>
@@ -29129,7 +29389,9 @@
       <c r="I184" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J184" s="33"/>
+      <c r="J184" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K184" s="33" t="s">
         <v>942</v>
       </c>
@@ -29232,7 +29494,9 @@
       <c r="I185" s="33" t="s">
         <v>1706</v>
       </c>
-      <c r="J185" s="33"/>
+      <c r="J185" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K185" s="33" t="s">
         <v>942</v>
       </c>
@@ -29335,7 +29599,9 @@
       <c r="I186" s="52" t="s">
         <v>912</v>
       </c>
-      <c r="J186" s="33"/>
+      <c r="J186" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K186" s="33" t="s">
         <v>942</v>
       </c>
@@ -29438,7 +29704,9 @@
       <c r="I187" s="33" t="s">
         <v>1708</v>
       </c>
-      <c r="J187" s="33"/>
+      <c r="J187" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K187" s="33" t="s">
         <v>942</v>
       </c>
@@ -29541,7 +29809,9 @@
       <c r="I188" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J188" s="33"/>
+      <c r="J188" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K188" s="33" t="s">
         <v>942</v>
       </c>
@@ -29644,7 +29914,9 @@
       <c r="I189" s="33" t="s">
         <v>1710</v>
       </c>
-      <c r="J189" s="33"/>
+      <c r="J189" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K189" s="33" t="s">
         <v>942</v>
       </c>
@@ -29747,7 +30019,9 @@
       <c r="I190" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J190" s="33"/>
+      <c r="J190" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K190" s="33" t="s">
         <v>942</v>
       </c>
@@ -29850,7 +30124,9 @@
       <c r="I191" s="33" t="s">
         <v>1712</v>
       </c>
-      <c r="J191" s="33"/>
+      <c r="J191" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K191" s="33" t="s">
         <v>942</v>
       </c>
@@ -29953,7 +30229,9 @@
       <c r="I192" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J192" s="33"/>
+      <c r="J192" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K192" s="33" t="s">
         <v>942</v>
       </c>
@@ -30056,7 +30334,9 @@
       <c r="I193" s="33" t="s">
         <v>1714</v>
       </c>
-      <c r="J193" s="33"/>
+      <c r="J193" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K193" s="33" t="s">
         <v>942</v>
       </c>
@@ -30159,7 +30439,9 @@
       <c r="I194" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J194" s="33"/>
+      <c r="J194" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K194" s="33" t="s">
         <v>942</v>
       </c>
@@ -30262,7 +30544,9 @@
       <c r="I195" s="33" t="s">
         <v>1716</v>
       </c>
-      <c r="J195" s="33"/>
+      <c r="J195" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K195" s="33" t="s">
         <v>942</v>
       </c>
@@ -30365,7 +30649,9 @@
       <c r="I196" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J196" s="33"/>
+      <c r="J196" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K196" s="33" t="s">
         <v>942</v>
       </c>
@@ -30468,7 +30754,9 @@
       <c r="I197" s="33" t="s">
         <v>1718</v>
       </c>
-      <c r="J197" s="33"/>
+      <c r="J197" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K197" s="33" t="s">
         <v>942</v>
       </c>
@@ -30571,7 +30859,9 @@
       <c r="I198" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J198" s="33"/>
+      <c r="J198" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K198" s="33" t="s">
         <v>942</v>
       </c>
@@ -30674,7 +30964,9 @@
       <c r="I199" s="33" t="s">
         <v>1720</v>
       </c>
-      <c r="J199" s="33"/>
+      <c r="J199" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K199" s="33" t="s">
         <v>942</v>
       </c>
@@ -30777,7 +31069,9 @@
       <c r="I200" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J200" s="33"/>
+      <c r="J200" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K200" s="33" t="s">
         <v>942</v>
       </c>
@@ -30880,7 +31174,9 @@
       <c r="I201" s="33" t="s">
         <v>1722</v>
       </c>
-      <c r="J201" s="33"/>
+      <c r="J201" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K201" s="33" t="s">
         <v>942</v>
       </c>
@@ -30983,7 +31279,9 @@
       <c r="I202" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J202" s="33"/>
+      <c r="J202" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K202" s="33" t="s">
         <v>942</v>
       </c>
@@ -31086,7 +31384,9 @@
       <c r="I203" s="33" t="s">
         <v>1724</v>
       </c>
-      <c r="J203" s="33"/>
+      <c r="J203" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K203" s="33" t="s">
         <v>942</v>
       </c>
@@ -31189,7 +31489,9 @@
       <c r="I204" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J204" s="33"/>
+      <c r="J204" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K204" s="33" t="s">
         <v>942</v>
       </c>
@@ -31292,7 +31594,9 @@
       <c r="I205" s="53" t="s">
         <v>1729</v>
       </c>
-      <c r="J205" s="33"/>
+      <c r="J205" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K205" s="33" t="s">
         <v>942</v>
       </c>
@@ -31395,7 +31699,9 @@
       <c r="I206" s="53" t="s">
         <v>912</v>
       </c>
-      <c r="J206" s="33"/>
+      <c r="J206" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K206" s="33" t="s">
         <v>942</v>
       </c>
@@ -31498,7 +31804,9 @@
       <c r="I207" s="53" t="s">
         <v>1730</v>
       </c>
-      <c r="J207" s="33"/>
+      <c r="J207" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K207" s="33" t="s">
         <v>942</v>
       </c>
@@ -31601,7 +31909,9 @@
       <c r="I208" s="53" t="s">
         <v>912</v>
       </c>
-      <c r="J208" s="33"/>
+      <c r="J208" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K208" s="33" t="s">
         <v>942</v>
       </c>
@@ -31704,7 +32014,9 @@
       <c r="I209" s="53" t="s">
         <v>1731</v>
       </c>
-      <c r="J209" s="33"/>
+      <c r="J209" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K209" s="33" t="s">
         <v>942</v>
       </c>
@@ -31807,7 +32119,9 @@
       <c r="I210" s="53" t="s">
         <v>912</v>
       </c>
-      <c r="J210" s="33"/>
+      <c r="J210" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K210" s="33" t="s">
         <v>942</v>
       </c>
@@ -31910,7 +32224,9 @@
       <c r="I211" s="53" t="s">
         <v>1732</v>
       </c>
-      <c r="J211" s="33"/>
+      <c r="J211" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K211" s="33" t="s">
         <v>942</v>
       </c>
@@ -32013,7 +32329,9 @@
       <c r="I212" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J212" s="33"/>
+      <c r="J212" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K212" s="33" t="s">
         <v>942</v>
       </c>
@@ -32116,7 +32434,9 @@
       <c r="I213" s="53" t="s">
         <v>1734</v>
       </c>
-      <c r="J213" s="33"/>
+      <c r="J213" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K213" s="33" t="s">
         <v>942</v>
       </c>
@@ -32219,7 +32539,9 @@
       <c r="I214" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J214" s="33"/>
+      <c r="J214" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K214" s="33" t="s">
         <v>942</v>
       </c>
@@ -32322,7 +32644,9 @@
       <c r="I215" s="54" t="s">
         <v>1736</v>
       </c>
-      <c r="J215" s="33"/>
+      <c r="J215" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K215" s="33" t="s">
         <v>942</v>
       </c>
@@ -32425,7 +32749,9 @@
       <c r="I216" s="55" t="s">
         <v>912</v>
       </c>
-      <c r="J216" s="33"/>
+      <c r="J216" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K216" s="33" t="s">
         <v>942</v>
       </c>
@@ -32528,7 +32854,9 @@
       <c r="I217" s="54" t="s">
         <v>1738</v>
       </c>
-      <c r="J217" s="33"/>
+      <c r="J217" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K217" s="33" t="s">
         <v>942</v>
       </c>
@@ -32631,7 +32959,9 @@
       <c r="I218" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J218" s="33"/>
+      <c r="J218" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K218" s="33" t="s">
         <v>942</v>
       </c>
@@ -32734,7 +33064,9 @@
       <c r="I219" s="54" t="s">
         <v>1740</v>
       </c>
-      <c r="J219" s="33"/>
+      <c r="J219" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K219" s="33" t="s">
         <v>942</v>
       </c>
@@ -32837,7 +33169,9 @@
       <c r="I220" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J220" s="33"/>
+      <c r="J220" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K220" s="33" t="s">
         <v>942</v>
       </c>
@@ -32940,7 +33274,9 @@
       <c r="I221" s="33" t="s">
         <v>1742</v>
       </c>
-      <c r="J221" s="33"/>
+      <c r="J221" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K221" s="33" t="s">
         <v>942</v>
       </c>
@@ -33043,7 +33379,9 @@
       <c r="I222" s="33" t="s">
         <v>1743</v>
       </c>
-      <c r="J222" s="33"/>
+      <c r="J222" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K222" s="33" t="s">
         <v>942</v>
       </c>
@@ -33146,7 +33484,9 @@
       <c r="I223" s="33" t="s">
         <v>1745</v>
       </c>
-      <c r="J223" s="33"/>
+      <c r="J223" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K223" s="33" t="s">
         <v>942</v>
       </c>
@@ -33249,7 +33589,9 @@
       <c r="I224" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J224" s="33"/>
+      <c r="J224" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K224" s="33" t="s">
         <v>942</v>
       </c>
@@ -33352,7 +33694,9 @@
       <c r="I225" s="54" t="s">
         <v>1748</v>
       </c>
-      <c r="J225" s="33"/>
+      <c r="J225" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K225" s="33" t="s">
         <v>942</v>
       </c>
@@ -33455,7 +33799,9 @@
       <c r="I226" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J226" s="33"/>
+      <c r="J226" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K226" s="33" t="s">
         <v>942</v>
       </c>
@@ -33558,7 +33904,9 @@
       <c r="I227" s="54" t="s">
         <v>1749</v>
       </c>
-      <c r="J227" s="33"/>
+      <c r="J227" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K227" s="33" t="s">
         <v>942</v>
       </c>
@@ -33661,7 +34009,9 @@
       <c r="I228" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J228" s="33"/>
+      <c r="J228" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K228" s="33" t="s">
         <v>942</v>
       </c>
@@ -33764,7 +34114,9 @@
       <c r="I229" s="54" t="s">
         <v>1751</v>
       </c>
-      <c r="J229" s="33"/>
+      <c r="J229" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K229" s="33" t="s">
         <v>942</v>
       </c>
@@ -33867,7 +34219,9 @@
       <c r="I230" s="56" t="s">
         <v>912</v>
       </c>
-      <c r="J230" s="33"/>
+      <c r="J230" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K230" s="33" t="s">
         <v>942</v>
       </c>
@@ -33970,7 +34324,9 @@
       <c r="I231" s="54" t="s">
         <v>1753</v>
       </c>
-      <c r="J231" s="33"/>
+      <c r="J231" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K231" s="33" t="s">
         <v>942</v>
       </c>
@@ -34073,7 +34429,9 @@
       <c r="I232" s="55" t="s">
         <v>912</v>
       </c>
-      <c r="J232" s="33"/>
+      <c r="J232" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K232" s="33" t="s">
         <v>942</v>
       </c>
@@ -34176,7 +34534,9 @@
       <c r="I233" s="54" t="s">
         <v>1755</v>
       </c>
-      <c r="J233" s="33"/>
+      <c r="J233" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K233" s="33" t="s">
         <v>942</v>
       </c>
@@ -34279,7 +34639,9 @@
       <c r="I234" s="55" t="s">
         <v>912</v>
       </c>
-      <c r="J234" s="33"/>
+      <c r="J234" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K234" s="33" t="s">
         <v>942</v>
       </c>
@@ -34382,7 +34744,9 @@
       <c r="I235" s="54" t="s">
         <v>1777</v>
       </c>
-      <c r="J235" s="33"/>
+      <c r="J235" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K235" s="33" t="s">
         <v>942</v>
       </c>
@@ -34485,7 +34849,9 @@
       <c r="I236" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J236" s="33"/>
+      <c r="J236" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K236" s="33" t="s">
         <v>942</v>
       </c>
@@ -34588,7 +34954,9 @@
       <c r="I237" s="54" t="s">
         <v>1757</v>
       </c>
-      <c r="J237" s="33"/>
+      <c r="J237" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K237" s="33" t="s">
         <v>942</v>
       </c>
@@ -34691,7 +35059,9 @@
       <c r="I238" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J238" s="33"/>
+      <c r="J238" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K238" s="33" t="s">
         <v>942</v>
       </c>
@@ -34794,7 +35164,9 @@
       <c r="I239" s="54" t="s">
         <v>1759</v>
       </c>
-      <c r="J239" s="33"/>
+      <c r="J239" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K239" s="33" t="s">
         <v>942</v>
       </c>
@@ -34897,7 +35269,9 @@
       <c r="I240" s="33" t="s">
         <v>1760</v>
       </c>
-      <c r="J240" s="33"/>
+      <c r="J240" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K240" s="33" t="s">
         <v>942</v>
       </c>
@@ -35000,7 +35374,9 @@
       <c r="I241" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J241" s="33"/>
+      <c r="J241" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K241" s="33" t="s">
         <v>942</v>
       </c>
@@ -35103,7 +35479,9 @@
       <c r="I242" s="54" t="s">
         <v>1761</v>
       </c>
-      <c r="J242" s="33"/>
+      <c r="J242" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K242" s="33" t="s">
         <v>942</v>
       </c>
@@ -35206,7 +35584,9 @@
       <c r="I243" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J243" s="33"/>
+      <c r="J243" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K243" s="33" t="s">
         <v>942</v>
       </c>
@@ -35309,7 +35689,9 @@
       <c r="I244" s="54" t="s">
         <v>1764</v>
       </c>
-      <c r="J244" s="33"/>
+      <c r="J244" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K244" s="33" t="s">
         <v>942</v>
       </c>
@@ -35412,7 +35794,9 @@
       <c r="I245" s="33" t="s">
         <v>912</v>
       </c>
-      <c r="J245" s="33"/>
+      <c r="J245" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K245" s="33" t="s">
         <v>942</v>
       </c>
@@ -35515,7 +35899,9 @@
       <c r="I246" s="54" t="s">
         <v>1776</v>
       </c>
-      <c r="J246" s="33"/>
+      <c r="J246" s="33" t="s">
+        <v>912</v>
+      </c>
       <c r="K246" s="33" t="s">
         <v>942</v>
       </c>

</xml_diff>

<commit_message>
fix a operation error
月の大小に誤りがあった
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC174AE-DF5B-7B47-B960-F578A2FC5530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC88995-3E55-9045-8868-C58865989043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="500" windowWidth="32100" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12292,10 +12292,10 @@
   <dimension ref="A1:AG489"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H464" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B473" sqref="B473"/>
+      <selection pane="bottomRight" activeCell="P98" sqref="P98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="20" customHeight="1"/>
@@ -22642,7 +22642,7 @@
         <v>640</v>
       </c>
       <c r="P98" s="31" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="Q98" s="31" t="s">
         <v>886</v>

</xml_diff>

<commit_message>
fix operation data '永承5年11月'
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC88995-3E55-9045-8868-C58865989043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC56301B-41A8-4045-B720-CD2F28A3E92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="500" windowWidth="32100" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11671" uniqueCount="2100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11671" uniqueCount="2101">
   <si>
     <t>ID</t>
   </si>
@@ -10484,6 +10484,10 @@
     <rPh sb="3" eb="4">
       <t>ガテゥ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1050-11-17</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -12292,10 +12296,10 @@
   <dimension ref="A1:AG489"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="J345" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P98" sqref="P98"/>
+      <selection pane="bottomRight" activeCell="W354" sqref="W354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="20" customHeight="1"/>
@@ -49796,7 +49800,7 @@
         <v>20</v>
       </c>
       <c r="V354" s="31" t="s">
-        <v>242</v>
+        <v>2100</v>
       </c>
       <c r="W354" s="31" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
fix '同治4年8月' operation setting
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F58C71-7912-4344-A4F4-895652E4EB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CC2836-4EB9-9C42-BC1B-B8A43C543AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="500" windowWidth="32100" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12287,10 +12287,10 @@
   <dimension ref="A1:AG488"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H432" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H360" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N434" sqref="N434"/>
+      <selection pane="bottomRight" activeCell="O368" sqref="O368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="20" customHeight="1"/>
@@ -51254,7 +51254,7 @@
         <v>2093</v>
       </c>
       <c r="O368" s="31" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="P368" s="31" t="s">
         <v>640</v>

</xml_diff>

<commit_message>
fix '寛治3年1月' operation setting
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8316D402-5B4D-0A46-A682-5511CE450B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE769285-2D8D-CC4A-8BAE-0054ECE35040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="500" windowWidth="32100" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12278,10 +12278,10 @@
   <dimension ref="A1:AG488"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H389" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H358" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H392" sqref="H392"/>
+      <selection pane="bottomRight" activeCell="O364" sqref="O364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="20" customHeight="1"/>
@@ -50821,7 +50821,7 @@
         <v>20</v>
       </c>
       <c r="O364" s="31" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="P364" s="31" t="s">
         <v>640</v>

</xml_diff>

<commit_message>
fix '天長2年12月' operation setting
</commit_message>
<xml_diff>
--- a/doc/operation/operation.xlsx
+++ b/doc/operation/operation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE769285-2D8D-CC4A-8BAE-0054ECE35040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95FAC17-E65C-534D-AB96-46DCF9E8C21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="500" windowWidth="32100" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9129,10 +9129,6 @@
   </si>
   <si>
     <t>天長 2年 12 大 己亥 35-1289</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>825-1-12</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -10470,6 +10466,10 @@
   </si>
   <si>
     <t>1228-1-9</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>826-1-12</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -12278,10 +12278,10 @@
   <dimension ref="A1:AG488"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H358" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H196" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O364" sqref="O364"/>
+      <selection pane="bottomRight" activeCell="H202" sqref="H202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="20" customHeight="1"/>
@@ -21017,7 +21017,7 @@
         <v>1556</v>
       </c>
       <c r="I83" s="31" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="J83" s="31" t="s">
         <v>882</v>
@@ -21950,7 +21950,7 @@
     <row r="92" spans="1:33" ht="48.5" customHeight="1">
       <c r="A92" s="66"/>
       <c r="B92" s="33" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C92" s="33" t="s">
         <v>882</v>
@@ -22056,7 +22056,7 @@
     <row r="93" spans="1:33" ht="48.5" customHeight="1">
       <c r="A93" s="66"/>
       <c r="B93" s="33" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C93" s="33" t="s">
         <v>882</v>
@@ -22162,7 +22162,7 @@
     <row r="94" spans="1:33" ht="48.5" customHeight="1">
       <c r="A94" s="66"/>
       <c r="B94" s="33" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C94" s="33" t="s">
         <v>882</v>
@@ -24088,7 +24088,7 @@
         <v>1919</v>
       </c>
       <c r="H112" s="36" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="I112" s="31" t="s">
         <v>882</v>
@@ -24176,7 +24176,7 @@
     <row r="113" spans="1:33" ht="48.5" customHeight="1">
       <c r="A113" s="66"/>
       <c r="B113" s="33" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C113" s="33" t="s">
         <v>882</v>
@@ -24282,7 +24282,7 @@
     <row r="114" spans="1:33" ht="48.5" customHeight="1">
       <c r="A114" s="66"/>
       <c r="B114" s="33" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C114" s="33" t="s">
         <v>882</v>
@@ -25766,7 +25766,7 @@
     <row r="128" spans="1:33" ht="48.5" customHeight="1">
       <c r="A128" s="66"/>
       <c r="B128" s="33" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="C128" s="33" t="s">
         <v>882</v>
@@ -25872,7 +25872,7 @@
     <row r="129" spans="1:33" ht="48.5" customHeight="1">
       <c r="A129" s="66"/>
       <c r="B129" s="33" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C129" s="33" t="s">
         <v>882</v>
@@ -25944,7 +25944,7 @@
         <v>1921</v>
       </c>
       <c r="Z129" s="31" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="AA129" s="32">
         <f>IF(W129="-","-",VLOOKUP(W129,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -27110,7 +27110,7 @@
         <v>1933</v>
       </c>
       <c r="Z140" s="31" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="AA140" s="32">
         <f>IF(W140="-","-",VLOOKUP(W140,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -27144,7 +27144,7 @@
     <row r="141" spans="1:33" ht="48.5" customHeight="1">
       <c r="A141" s="66"/>
       <c r="B141" s="33" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="C141" s="33" t="s">
         <v>882</v>
@@ -27159,7 +27159,7 @@
         <v>882</v>
       </c>
       <c r="G141" s="35" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="H141" s="36" t="s">
         <v>1941</v>
@@ -27322,7 +27322,7 @@
         <v>1943</v>
       </c>
       <c r="Z142" s="31" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="AA142" s="32">
         <f>IF(W142="-","-",VLOOKUP(W142,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -27462,7 +27462,7 @@
     <row r="144" spans="1:33" ht="48.5" customHeight="1">
       <c r="A144" s="66"/>
       <c r="B144" s="33" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="C144" s="33" t="s">
         <v>882</v>
@@ -27568,13 +27568,13 @@
     <row r="145" spans="1:33" ht="48.5" customHeight="1">
       <c r="A145" s="66"/>
       <c r="B145" s="33" t="s">
+        <v>2033</v>
+      </c>
+      <c r="C145" s="33" t="s">
+        <v>882</v>
+      </c>
+      <c r="D145" s="33" t="s">
         <v>2034</v>
-      </c>
-      <c r="C145" s="33" t="s">
-        <v>882</v>
-      </c>
-      <c r="D145" s="33" t="s">
-        <v>2035</v>
       </c>
       <c r="E145" s="34">
         <v>130</v>
@@ -27674,7 +27674,7 @@
     <row r="146" spans="1:33" ht="48.5" customHeight="1">
       <c r="A146" s="66"/>
       <c r="B146" s="33" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C146" s="33" t="s">
         <v>882</v>
@@ -27780,13 +27780,13 @@
     <row r="147" spans="1:33" ht="48.5" customHeight="1">
       <c r="A147" s="66"/>
       <c r="B147" s="33" t="s">
+        <v>2035</v>
+      </c>
+      <c r="C147" s="33" t="s">
+        <v>882</v>
+      </c>
+      <c r="D147" s="33" t="s">
         <v>2036</v>
-      </c>
-      <c r="C147" s="33" t="s">
-        <v>882</v>
-      </c>
-      <c r="D147" s="33" t="s">
-        <v>2037</v>
       </c>
       <c r="E147" s="34">
         <v>130</v>
@@ -27886,7 +27886,7 @@
     <row r="148" spans="1:33" ht="48.5" customHeight="1">
       <c r="A148" s="66"/>
       <c r="B148" s="33" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C148" s="33" t="s">
         <v>882</v>
@@ -30396,7 +30396,7 @@
         <v>1954</v>
       </c>
       <c r="Z171" s="31" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="AA171" s="32">
         <f>IF(W171="-","-",VLOOKUP(W171,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -30608,7 +30608,7 @@
         <v>1961</v>
       </c>
       <c r="Z173" s="31" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="AA173" s="32">
         <f>IF(W173="-","-",VLOOKUP(W173,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -31596,7 +31596,7 @@
     <row r="183" spans="1:33" ht="48.5" customHeight="1">
       <c r="A183" s="66"/>
       <c r="B183" s="33" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="C183" s="51" t="s">
         <v>882</v>
@@ -31774,7 +31774,7 @@
         <v>1972</v>
       </c>
       <c r="Z184" s="31" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="AA184" s="32">
         <f>IF(W184="-","-",VLOOKUP(W184,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -33625,7 +33625,7 @@
         <v>882</v>
       </c>
       <c r="G202" s="35" t="s">
-        <v>1991</v>
+        <v>2097</v>
       </c>
       <c r="H202" s="38" t="s">
         <v>1990</v>
@@ -33737,7 +33737,7 @@
         <v>1800</v>
       </c>
       <c r="I203" s="31" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="J203" s="31" t="s">
         <v>882</v>
@@ -33943,10 +33943,10 @@
         <v>892</v>
       </c>
       <c r="G205" s="35" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="H205" s="56" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="I205" s="55" t="s">
         <v>882</v>
@@ -34034,7 +34034,7 @@
     <row r="206" spans="1:33" ht="48.5" customHeight="1">
       <c r="A206" s="66"/>
       <c r="B206" s="33" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C206" s="33" t="s">
         <v>882</v>
@@ -34052,7 +34052,7 @@
         <v>1297</v>
       </c>
       <c r="H206" s="36" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="I206" s="31" t="s">
         <v>882</v>
@@ -34140,13 +34140,13 @@
     <row r="207" spans="1:33" ht="48.5" customHeight="1">
       <c r="A207" s="66"/>
       <c r="B207" s="33" t="s">
+        <v>2043</v>
+      </c>
+      <c r="C207" s="33" t="s">
+        <v>882</v>
+      </c>
+      <c r="D207" s="33" t="s">
         <v>2044</v>
-      </c>
-      <c r="C207" s="33" t="s">
-        <v>882</v>
-      </c>
-      <c r="D207" s="33" t="s">
-        <v>2045</v>
       </c>
       <c r="E207" s="34">
         <v>141</v>
@@ -34246,7 +34246,7 @@
     <row r="208" spans="1:33" ht="48.5" customHeight="1">
       <c r="A208" s="66"/>
       <c r="B208" s="33" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="C208" s="33" t="s">
         <v>882</v>
@@ -34267,7 +34267,7 @@
         <v>1609</v>
       </c>
       <c r="I208" s="31" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="J208" s="31" t="s">
         <v>882</v>
@@ -34352,7 +34352,7 @@
     <row r="209" spans="1:33" ht="48.5" customHeight="1">
       <c r="A209" s="66"/>
       <c r="B209" s="33" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="C209" s="33" t="s">
         <v>882</v>
@@ -34373,7 +34373,7 @@
         <v>1610</v>
       </c>
       <c r="I209" s="31" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="J209" s="31" t="s">
         <v>882</v>
@@ -34458,7 +34458,7 @@
     <row r="210" spans="1:33" ht="48.5" customHeight="1">
       <c r="A210" s="66"/>
       <c r="B210" s="33" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C210" s="33" t="s">
         <v>882</v>
@@ -34479,7 +34479,7 @@
         <v>1611</v>
       </c>
       <c r="I210" s="31" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="J210" s="31" t="s">
         <v>882</v>
@@ -34564,13 +34564,13 @@
     <row r="211" spans="1:33" ht="48.5" customHeight="1">
       <c r="A211" s="66"/>
       <c r="B211" s="33" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C211" s="51" t="s">
         <v>882</v>
       </c>
       <c r="D211" s="33" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="E211" s="34">
         <v>141</v>
@@ -34579,10 +34579,10 @@
         <v>882</v>
       </c>
       <c r="G211" s="54" t="s">
+        <v>1998</v>
+      </c>
+      <c r="H211" s="36" t="s">
         <v>1999</v>
-      </c>
-      <c r="H211" s="36" t="s">
-        <v>2000</v>
       </c>
       <c r="I211" s="55" t="s">
         <v>882</v>
@@ -34670,7 +34670,7 @@
     <row r="212" spans="1:33" ht="48.5" customHeight="1">
       <c r="A212" s="66"/>
       <c r="B212" s="33" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="C212" s="33" t="s">
         <v>882</v>
@@ -34685,13 +34685,13 @@
         <v>898</v>
       </c>
       <c r="G212" s="35" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="H212" s="36" t="s">
+        <v>2000</v>
+      </c>
+      <c r="I212" s="55" t="s">
         <v>2001</v>
-      </c>
-      <c r="I212" s="55" t="s">
-        <v>2002</v>
       </c>
       <c r="J212" s="55" t="s">
         <v>882</v>
@@ -34739,10 +34739,10 @@
         <v>1973</v>
       </c>
       <c r="Y212" s="31" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="Z212" s="31" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="AA212" s="32">
         <f>IF(W212="-","-",VLOOKUP(W212,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -34903,7 +34903,7 @@
         <v>1612</v>
       </c>
       <c r="I214" s="31" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="J214" s="31" t="s">
         <v>882</v>
@@ -35094,7 +35094,7 @@
     <row r="216" spans="1:33" ht="48.5" customHeight="1">
       <c r="A216" s="66"/>
       <c r="B216" s="33" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C216" s="51" t="s">
         <v>882</v>
@@ -35109,10 +35109,10 @@
         <v>882</v>
       </c>
       <c r="G216" s="54" t="s">
+        <v>2007</v>
+      </c>
+      <c r="H216" s="36" t="s">
         <v>2008</v>
-      </c>
-      <c r="H216" s="36" t="s">
-        <v>2009</v>
       </c>
       <c r="I216" s="55" t="s">
         <v>882</v>
@@ -35215,13 +35215,13 @@
         <v>901</v>
       </c>
       <c r="G217" s="35" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H217" s="36" t="s">
+        <v>2009</v>
+      </c>
+      <c r="I217" s="55" t="s">
         <v>2010</v>
-      </c>
-      <c r="I217" s="55" t="s">
-        <v>2011</v>
       </c>
       <c r="J217" s="55" t="s">
         <v>882</v>
@@ -35230,7 +35230,7 @@
         <v>912</v>
       </c>
       <c r="L217" s="55" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="M217" s="31" t="s">
         <v>20</v>
@@ -35263,16 +35263,16 @@
         <v>20</v>
       </c>
       <c r="W217" s="31" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="X217" s="31" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="Y217" s="31" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="Z217" s="31" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="AA217" s="32">
         <f>IF(W217="-","-",VLOOKUP(W217,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -35430,10 +35430,10 @@
         <v>1306</v>
       </c>
       <c r="H219" s="36" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="I219" s="58" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="J219" s="31" t="s">
         <v>882</v>
@@ -35518,7 +35518,7 @@
     <row r="220" spans="1:33" ht="48.5" customHeight="1">
       <c r="A220" s="66"/>
       <c r="B220" s="51" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="C220" s="51" t="s">
         <v>1035</v>
@@ -35533,10 +35533,10 @@
         <v>901</v>
       </c>
       <c r="G220" s="54" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="H220" s="36" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I220" s="58" t="s">
         <v>882</v>
@@ -35548,7 +35548,7 @@
         <v>912</v>
       </c>
       <c r="L220" s="55" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="M220" s="31" t="s">
         <v>882</v>
@@ -35587,10 +35587,10 @@
         <v>1893</v>
       </c>
       <c r="Y220" s="31" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="Z220" s="31" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="AA220" s="32">
         <f>IF(W220="-","-",VLOOKUP(W220,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -42520,7 +42520,7 @@
         <v>20</v>
       </c>
       <c r="D286" s="33" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E286" s="34">
         <v>156</v>
@@ -42620,7 +42620,7 @@
     <row r="287" spans="1:33" ht="48.25" customHeight="1">
       <c r="A287" s="66"/>
       <c r="B287" s="51" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C287" s="33" t="s">
         <v>20</v>
@@ -45715,7 +45715,7 @@
         <v>126</v>
       </c>
       <c r="I316" s="31" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="J316" s="31" t="s">
         <v>20</v>
@@ -45818,7 +45818,7 @@
         <v>681</v>
       </c>
       <c r="H317" s="36" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="I317" s="31" t="s">
         <v>20</v>
@@ -47944,7 +47944,7 @@
         <v>192</v>
       </c>
       <c r="J337" s="31" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="K337" s="31" t="s">
         <v>637</v>
@@ -48156,7 +48156,7 @@
         <v>199</v>
       </c>
       <c r="J339" s="31" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="K339" s="31" t="s">
         <v>637</v>
@@ -48789,7 +48789,7 @@
         <v>214</v>
       </c>
       <c r="I345" s="31" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="J345" s="31" t="s">
         <v>20</v>
@@ -49782,7 +49782,7 @@
         <v>20</v>
       </c>
       <c r="V354" s="31" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="W354" s="31" t="s">
         <v>85</v>
@@ -49934,13 +49934,13 @@
     <row r="356" spans="1:33" ht="33.25" customHeight="1">
       <c r="A356" s="66"/>
       <c r="B356" s="33" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="C356" s="33" t="s">
         <v>882</v>
       </c>
       <c r="D356" s="33" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="E356" s="34">
         <v>220</v>
@@ -49949,10 +49949,10 @@
         <v>882</v>
       </c>
       <c r="G356" s="35" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="H356" s="36" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="I356" s="31" t="s">
         <v>882</v>
@@ -50040,7 +50040,7 @@
     <row r="357" spans="1:33" ht="33.25" customHeight="1">
       <c r="A357" s="66"/>
       <c r="B357" s="33" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="C357" s="33" t="s">
         <v>882</v>
@@ -50055,13 +50055,13 @@
         <v>1</v>
       </c>
       <c r="G357" s="35" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="H357" s="36" t="s">
+        <v>2062</v>
+      </c>
+      <c r="I357" s="31" t="s">
         <v>2063</v>
-      </c>
-      <c r="I357" s="31" t="s">
-        <v>2064</v>
       </c>
       <c r="J357" s="31" t="s">
         <v>882</v>
@@ -50109,10 +50109,10 @@
         <v>1805</v>
       </c>
       <c r="Y357" s="31" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="Z357" s="31" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="AA357" s="32">
         <f>IF(W357="-","-",VLOOKUP(W357,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -50464,13 +50464,13 @@
     <row r="361" spans="1:33" ht="33.25" customHeight="1">
       <c r="A361" s="66"/>
       <c r="B361" s="33" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C361" s="33" t="s">
+        <v>882</v>
+      </c>
+      <c r="D361" s="33" t="s">
         <v>2066</v>
-      </c>
-      <c r="C361" s="33" t="s">
-        <v>882</v>
-      </c>
-      <c r="D361" s="33" t="s">
-        <v>2067</v>
       </c>
       <c r="E361" s="34">
         <v>226</v>
@@ -50479,10 +50479,10 @@
         <v>882</v>
       </c>
       <c r="G361" s="35" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="H361" s="36" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="I361" s="31" t="s">
         <v>882</v>
@@ -50570,7 +50570,7 @@
     <row r="362" spans="1:33" ht="54">
       <c r="A362" s="66"/>
       <c r="B362" s="33" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="C362" s="33" t="s">
         <v>882</v>
@@ -50585,13 +50585,13 @@
         <v>1</v>
       </c>
       <c r="G362" s="35" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="H362" s="36" t="s">
+        <v>2070</v>
+      </c>
+      <c r="I362" s="31" t="s">
         <v>2071</v>
-      </c>
-      <c r="I362" s="31" t="s">
-        <v>2072</v>
       </c>
       <c r="J362" s="31" t="s">
         <v>882</v>
@@ -50639,10 +50639,10 @@
         <v>1988</v>
       </c>
       <c r="Y362" s="31" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="Z362" s="31" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="AA362" s="32">
         <f>IF(W362="-","-",VLOOKUP(W362,十干十二支!A$2:B$61,2,FALSE))</f>
@@ -51133,10 +51133,10 @@
         <v>645</v>
       </c>
       <c r="M367" s="31" t="s">
+        <v>2091</v>
+      </c>
+      <c r="N367" s="31" t="s">
         <v>2092</v>
-      </c>
-      <c r="N367" s="31" t="s">
-        <v>2093</v>
       </c>
       <c r="O367" s="31" t="s">
         <v>640</v>
@@ -51239,10 +51239,10 @@
         <v>748</v>
       </c>
       <c r="M368" s="31" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N368" s="31" t="s">
         <v>2091</v>
-      </c>
-      <c r="N368" s="31" t="s">
-        <v>2092</v>
       </c>
       <c r="O368" s="31" t="s">
         <v>639</v>
@@ -53765,7 +53765,7 @@
         <v>20</v>
       </c>
       <c r="G392" s="35" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="H392" s="36" t="s">
         <v>777</v>
@@ -55679,7 +55679,7 @@
         <v>388</v>
       </c>
       <c r="I410" s="31" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="J410" s="31" t="s">
         <v>20</v>
@@ -57481,7 +57481,7 @@
         <v>450</v>
       </c>
       <c r="I427" s="31" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="J427" s="31" t="s">
         <v>20</v>
@@ -57587,7 +57587,7 @@
         <v>20</v>
       </c>
       <c r="I428" s="31" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="J428" s="31" t="s">
         <v>20</v>
@@ -57905,7 +57905,7 @@
         <v>458</v>
       </c>
       <c r="I431" s="31" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="J431" s="31" t="s">
         <v>20</v>
@@ -58329,7 +58329,7 @@
         <v>470</v>
       </c>
       <c r="I435" s="31" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="J435" s="31" t="s">
         <v>20</v>
@@ -59280,7 +59280,7 @@
         <v>495</v>
       </c>
       <c r="H444" s="36" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="I444" s="31" t="s">
         <v>20</v>
@@ -60131,7 +60131,7 @@
         <v>519</v>
       </c>
       <c r="I452" s="31" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="J452" s="31" t="s">
         <v>882</v>
@@ -60449,7 +60449,7 @@
         <v>20</v>
       </c>
       <c r="I455" s="31" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="J455" s="31" t="s">
         <v>20</v>
@@ -61082,7 +61082,7 @@
         <v>847</v>
       </c>
       <c r="H461" s="36" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="I461" s="31" t="s">
         <v>20</v>
@@ -61403,7 +61403,7 @@
         <v>547</v>
       </c>
       <c r="I464" s="31" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="J464" s="31" t="s">
         <v>20</v>
@@ -61721,7 +61721,7 @@
         <v>558</v>
       </c>
       <c r="I467" s="31" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="J467" s="31" t="s">
         <v>20</v>
@@ -62157,7 +62157,7 @@
         <v>733</v>
       </c>
       <c r="M471" s="31" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="N471" s="31" t="s">
         <v>239</v>
@@ -62263,10 +62263,10 @@
         <v>733</v>
       </c>
       <c r="M472" s="31" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="N472" s="31" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="O472" s="31" t="s">
         <v>640</v>
@@ -62357,7 +62357,7 @@
         <v>20</v>
       </c>
       <c r="I473" s="31" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="J473" s="31" t="s">
         <v>20</v>
@@ -63417,7 +63417,7 @@
         <v>608</v>
       </c>
       <c r="I483" s="31" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="J483" s="31" t="s">
         <v>20</v>
@@ -63626,7 +63626,7 @@
         <v>612</v>
       </c>
       <c r="H485" s="36" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="I485" s="31" t="s">
         <v>20</v>
@@ -63732,10 +63732,10 @@
         <v>614</v>
       </c>
       <c r="H486" s="36" t="s">
+        <v>2087</v>
+      </c>
+      <c r="I486" s="31" t="s">
         <v>2088</v>
-      </c>
-      <c r="I486" s="31" t="s">
-        <v>2089</v>
       </c>
       <c r="J486" s="31" t="s">
         <v>20</v>
@@ -63947,7 +63947,7 @@
         <v>20</v>
       </c>
       <c r="I488" s="64" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="J488" s="64" t="s">
         <v>20</v>

</xml_diff>